<commit_message>
simple rna model transcription and degradation
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model.xlsx
+++ b/rand_wc_model_gen/model_gen/model.xlsx
@@ -45,9 +45,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$21</definedName>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="329">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-13 16:30:44</t>
+    <t>2019-08-14 13:49:08</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4535,6 +4535,15 @@
     <t>AMP</t>
   </si>
   <si>
+    <t>C1=NC(=C2C(=N1)N(C=N2)C3C(C(C(O3)COP(=O)([O-])[O-])O)O)N</t>
+  </si>
+  <si>
+    <t>smiles</t>
+  </si>
+  <si>
+    <t>C10H12N5O7P</t>
+  </si>
+  <si>
     <t>metabolite</t>
   </si>
   <si>
@@ -4544,6 +4553,12 @@
     <t>ATP</t>
   </si>
   <si>
+    <t>C1=NC(=C2C(=N1)N(C=N2)C3C(C(C(O3)COP(=O)([O-])OP(=O)([O-])OP(=O)([O-])[O-])O)O)N</t>
+  </si>
+  <si>
+    <t>C10H12N5O13P3</t>
+  </si>
+  <si>
     <t>atp_synthase</t>
   </si>
   <si>
@@ -4559,12 +4574,24 @@
     <t>CMP</t>
   </si>
   <si>
+    <t>C1=CN(C(=O)N=C1N)C2C(C(C(O2)COP(=O)([O-])[O-])O)O</t>
+  </si>
+  <si>
+    <t>C9H12N3O8P</t>
+  </si>
+  <si>
     <t>ctp</t>
   </si>
   <si>
     <t>CTP</t>
   </si>
   <si>
+    <t>C1=CN(C(=O)N=C1N)C2C(C(C(O2)COP(=O)([O-])OP(=O)([O-])OP(=O)([O-])[O-])O)O</t>
+  </si>
+  <si>
+    <t>C9H12N3O14P3</t>
+  </si>
+  <si>
     <t>ctp_synthase</t>
   </si>
   <si>
@@ -4577,12 +4604,24 @@
     <t>GMP</t>
   </si>
   <si>
+    <t>C1=NC2=C(N1C3C(C(C(O3)COP(=O)([O-])[O-])O)O)N=C(NC2=O)N</t>
+  </si>
+  <si>
+    <t>C10H12N5O8P</t>
+  </si>
+  <si>
     <t>gtp</t>
   </si>
   <si>
     <t>GTP</t>
   </si>
   <si>
+    <t>C1=NC2=C(N1C3C(C(C(O3)COP(=O)([O-])OP(=O)([O-])OP(=O)([O-])[O-])O)O)N=C(NC2=O)N</t>
+  </si>
+  <si>
+    <t>C10H12N5O14P3</t>
+  </si>
+  <si>
     <t>gtp_synthase</t>
   </si>
   <si>
@@ -4595,25 +4634,37 @@
     <t>H</t>
   </si>
   <si>
+    <t>[H+]</t>
+  </si>
+  <si>
     <t>h2o</t>
   </si>
   <si>
     <t>H2O</t>
   </si>
   <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>ppi</t>
   </si>
   <si>
     <t>PPi</t>
   </si>
   <si>
+    <t>OP(=O)([O-])OP(=O)([O-])[O-]</t>
+  </si>
+  <si>
+    <t>HO7P2</t>
+  </si>
+  <si>
     <t>rna_1</t>
   </si>
   <si>
     <t>RNA 1</t>
   </si>
   <si>
-    <t>AAUG</t>
+    <t>AAUGUGC</t>
   </si>
   <si>
     <t>bpforms</t>
@@ -4622,7 +4673,7 @@
     <t>rna</t>
   </si>
   <si>
-    <t>C39H44N17O28P4</t>
+    <t>C67H76N27O50P7</t>
   </si>
   <si>
     <t>RNA</t>
@@ -4646,7 +4697,10 @@
     <t>RNA 3</t>
   </si>
   <si>
-    <t>ACGU</t>
+    <t>ACGUC</t>
+  </si>
+  <si>
+    <t>C47H55N18O36P5</t>
   </si>
   <si>
     <t>rna_pol</t>
@@ -4667,12 +4721,24 @@
     <t>UMP</t>
   </si>
   <si>
+    <t>C1=CN(C(=O)NC1=O)C2C(C(C(O2)COP(=O)([O-])[O-])O)O</t>
+  </si>
+  <si>
+    <t>C9H11N2O9P</t>
+  </si>
+  <si>
     <t>utp</t>
   </si>
   <si>
     <t>UTP</t>
   </si>
   <si>
+    <t>C1=CN(C(=O)NC1=O)C2C(C(C(O2)COP(=O)([O-])OP(=O)([O-])OP(=O)([O-])[O-])O)O</t>
+  </si>
+  <si>
+    <t>C9H11N2O15P3</t>
+  </si>
+  <si>
     <t>utp_synthase</t>
   </si>
   <si>
@@ -4838,12 +4904,108 @@
     <t>Maximum</t>
   </si>
   <si>
+    <t>degradation_rna_1</t>
+  </si>
+  <si>
+    <t>degradation RNA 1</t>
+  </si>
+  <si>
+    <t>[c]: (6) h2o + rna_1 ==&gt; (2) amp + cmp + (2) gmp + (6) h + (2) ump</t>
+  </si>
+  <si>
+    <t>1 / second</t>
+  </si>
+  <si>
+    <t>degradation_rna_2</t>
+  </si>
+  <si>
+    <t>degradation RNA 2</t>
+  </si>
+  <si>
+    <t>[c]: (3) h2o + rna_2 ==&gt; amp + cmp + gmp + (3) h + ump</t>
+  </si>
+  <si>
+    <t>degradation_rna_3</t>
+  </si>
+  <si>
+    <t>degradation RNA 3</t>
+  </si>
+  <si>
+    <t>[c]: (4) h2o + rna_3 ==&gt; amp + (2) cmp + gmp + (4) h + ump</t>
+  </si>
+  <si>
+    <t>transcription_rna_1</t>
+  </si>
+  <si>
+    <t>transcription RNA 1</t>
+  </si>
+  <si>
+    <t>[c]: (2) atp + ctp + (2) gtp + h2o + (2) utp ==&gt; h + (7) ppi + rna_1</t>
+  </si>
+  <si>
+    <t>transcription_rna_2</t>
+  </si>
+  <si>
+    <t>transcription RNA 2</t>
+  </si>
+  <si>
+    <t>[c]: atp + ctp + gtp + h2o + utp ==&gt; h + (4) ppi + rna_2</t>
+  </si>
+  <si>
+    <t>transcription_rna_3</t>
+  </si>
+  <si>
+    <t>transcription RNA 3</t>
+  </si>
+  <si>
+    <t>[c]: atp + (2) ctp + gtp + h2o + utp ==&gt; h + (5) ppi + rna_3</t>
+  </si>
+  <si>
     <t>Reaction</t>
   </si>
   <si>
     <t>Direction</t>
   </si>
   <si>
+    <t>degradation_rna_1-forward</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_1 * rna_1[c] / (km_deg_rna_1 * Avogadro * volume_c + rna_1[c])</t>
+  </si>
+  <si>
+    <t>degradation_rna_2-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_2 * rna_2[c] / (km_deg_rna_2 * Avogadro * volume_c + rna_2[c])</t>
+  </si>
+  <si>
+    <t>degradation_rna_3-forward</t>
+  </si>
+  <si>
+    <t>k_deg_rna_3 * rna_3[c] / (km_deg_rna_3 * Avogadro * volume_c + rna_3[c])</t>
+  </si>
+  <si>
+    <t>transcription_rna_1-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_1 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c]))</t>
+  </si>
+  <si>
+    <t>transcription_rna_2-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_2 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c]))</t>
+  </si>
+  <si>
+    <t>transcription_rna_3-forward</t>
+  </si>
+  <si>
+    <t>k_trans_rna_3 * (atp[c] / (km_atp_trans * Avogadro * volume_c + atp[c])) * (gtp[c] / (km_gtp_trans * Avogadro * volume_c + gtp[c])) * (ctp[c] / (km_ctp_trans * Avogadro * volume_c + ctp[c])) * (utp[c] / (km_utp_trans * Avogadro * volume_c + utp[c]))</t>
+  </si>
+  <si>
     <t>Reaction rate units</t>
   </si>
   <si>
@@ -4878,6 +5040,54 @@
   </si>
   <si>
     <t>half_life_rna_3</t>
+  </si>
+  <si>
+    <t>k_deg_rna_1</t>
+  </si>
+  <si>
+    <t>k_cat</t>
+  </si>
+  <si>
+    <t>k_deg_rna_2</t>
+  </si>
+  <si>
+    <t>k_deg_rna_3</t>
+  </si>
+  <si>
+    <t>k_trans_rna_1</t>
+  </si>
+  <si>
+    <t>k_trans_rna_2</t>
+  </si>
+  <si>
+    <t>k_trans_rna_3</t>
+  </si>
+  <si>
+    <t>km_atp_trans</t>
+  </si>
+  <si>
+    <t>K_m</t>
+  </si>
+  <si>
+    <t>molar</t>
+  </si>
+  <si>
+    <t>km_ctp_trans</t>
+  </si>
+  <si>
+    <t>km_deg_rna_1</t>
+  </si>
+  <si>
+    <t>km_deg_rna_2</t>
+  </si>
+  <si>
+    <t>km_deg_rna_3</t>
+  </si>
+  <si>
+    <t>km_gtp_trans</t>
+  </si>
+  <si>
+    <t>km_utp_trans</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -5493,7 +5703,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.01" customHeight="1">
@@ -5502,7 +5712,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.01" customHeight="1">
@@ -5538,7 +5748,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -5659,7 +5869,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -5731,7 +5941,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -5754,11 +5964,11 @@
     </row>
     <row r="2" spans="1:9" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>93</v>
@@ -5797,7 +6007,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -5818,13 +6028,13 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -5840,22 +6050,22 @@
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>84</v>
@@ -5876,47 +6086,215 @@
         <v>46</v>
       </c>
     </row>
+    <row r="3" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N2"/>
+  <autoFilter ref="A2:N8"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A3">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A8">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B3">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B8">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C2:C3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C8">
       <formula1>'Submodels'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D2:D3"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E2:E3">
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D8"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E8">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F2:F3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F8">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G2:G3">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G8">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H2:H3">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H8">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I2:I3">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I8">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J2:J3"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K2:K3"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L2:L3"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M2:M3">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J8"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L8"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M8">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N2:N3"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5925,7 +6303,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5946,16 +6324,16 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>84</v>
@@ -5976,36 +6354,180 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L1"/>
+  <autoFilter ref="A1:L7"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A1:A2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A7">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B1:B2">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B7">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C1:C2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C7">
       <formula1>'Reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D1:D2">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D7">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E1:E2">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E7">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F1:F2"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G1:G2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F7"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G7">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H1:H2"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I1:I2"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J1:J2"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K1:K2">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H7"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J7"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K7">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L1:L2"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6035,19 +6557,19 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>209</v>
+        <v>263</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>210</v>
+        <v>264</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -6124,13 +6646,13 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>211</v>
+        <v>265</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6204,7 +6726,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>212</v>
+        <v>266</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
@@ -6269,7 +6791,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6296,7 +6818,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>84</v>
@@ -6319,7 +6841,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6328,7 +6850,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>215</v>
+        <v>269</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6338,7 +6860,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6366,7 +6888,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>217</v>
+        <v>271</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6376,7 +6898,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6395,7 +6917,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>219</v>
+        <v>273</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6414,7 +6936,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>220</v>
+        <v>274</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6431,35 +6953,308 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
+    <row r="8" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.003850817669777474</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.003850817669777474</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.003850817669777474</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.03080654135821979</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.03080654135821979</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.03080654135821979</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K7"/>
+  <autoFilter ref="A1:K20"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A7">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A20">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B7">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B20">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C7">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C20">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D7">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D20">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E7">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E20">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G7"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I7"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J7">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F20"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G20"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H20"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I20"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J20">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K20"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6489,7 +7284,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -6561,10 +7356,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>221</v>
+        <v>291</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>221</v>
+        <v>291</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -6587,16 +7382,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>222</v>
+        <v>292</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>222</v>
+        <v>292</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -6613,7 +7408,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -6625,7 +7420,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>224</v>
+        <v>294</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -6637,19 +7432,19 @@
         <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>225</v>
+        <v>295</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>227</v>
+        <v>297</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>228</v>
+        <v>298</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>229</v>
+        <v>299</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -6979,10 +7774,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>230</v>
+        <v>300</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7002,7 +7797,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7032,7 +7827,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>231</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -7105,46 +7900,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>232</v>
+        <v>302</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>233</v>
+        <v>303</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>234</v>
+        <v>304</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>235</v>
+        <v>305</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>236</v>
+        <v>306</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>237</v>
+        <v>307</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>238</v>
+        <v>308</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>239</v>
+        <v>309</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>240</v>
+        <v>310</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>241</v>
+        <v>311</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>242</v>
+        <v>312</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>243</v>
+        <v>313</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>244</v>
+        <v>314</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -7239,28 +8034,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>246</v>
+        <v>316</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>247</v>
+        <v>317</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>232</v>
+        <v>302</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>248</v>
+        <v>318</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>249</v>
+        <v>319</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>250</v>
+        <v>320</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>251</v>
+        <v>321</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7343,25 +8138,25 @@
         <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>252</v>
+        <v>322</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>253</v>
+        <v>323</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>254</v>
+        <v>324</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>255</v>
+        <v>325</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>256</v>
+        <v>326</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>257</v>
+        <v>327</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>258</v>
+        <v>328</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -7382,7 +8177,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>231</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -7995,14 +8790,24 @@
       <c r="B3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="3">
+        <v>345.207761998</v>
+      </c>
+      <c r="H3" s="3">
+        <v>-2</v>
+      </c>
       <c r="I3" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -8012,19 +8817,29 @@
     </row>
     <row r="4" spans="1:14" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" s="3">
+        <v>503.149285994</v>
+      </c>
+      <c r="H4" s="3">
+        <v>-4</v>
+      </c>
       <c r="I4" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -8034,10 +8849,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -8046,7 +8861,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -8056,19 +8871,29 @@
     </row>
     <row r="6" spans="1:14" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="3">
+        <v>321.181761998</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-2</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -8078,19 +8903,29 @@
     </row>
     <row r="7" spans="1:14" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="3">
+        <v>479.123285994</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-4</v>
+      </c>
       <c r="I7" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -8100,10 +8935,10 @@
     </row>
     <row r="8" spans="1:14" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -8112,7 +8947,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -8122,19 +8957,29 @@
     </row>
     <row r="9" spans="1:14" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="3">
+        <v>361.206761998</v>
+      </c>
+      <c r="H9" s="3">
+        <v>-2</v>
+      </c>
       <c r="I9" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -8144,19 +8989,29 @@
     </row>
     <row r="10" spans="1:14" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+        <v>132</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="3">
+        <v>519.1482859939999</v>
+      </c>
+      <c r="H10" s="3">
+        <v>-4</v>
+      </c>
       <c r="I10" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -8166,10 +9021,10 @@
     </row>
     <row r="11" spans="1:14" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -8178,7 +9033,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -8188,19 +9043,29 @@
     </row>
     <row r="12" spans="1:14" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+        <v>138</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.008</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
       <c r="I12" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -8210,19 +9075,29 @@
     </row>
     <row r="13" spans="1:14" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="3">
+        <v>18.015</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
       <c r="I13" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -8232,19 +9107,29 @@
     </row>
     <row r="14" spans="1:14" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="3">
+        <v>174.948523996</v>
+      </c>
+      <c r="H14" s="3">
+        <v>-3</v>
+      </c>
       <c r="I14" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -8254,31 +9139,31 @@
     </row>
     <row r="15" spans="1:14" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="G15" s="3">
-        <v>1322.767047992</v>
+        <v>2276.300333986001</v>
       </c>
       <c r="H15" s="3">
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -8288,22 +9173,22 @@
     </row>
     <row r="16" spans="1:14" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="G16" s="3">
         <v>1298.741047992</v>
@@ -8312,7 +9197,7 @@
         <v>-5</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -8322,31 +9207,31 @@
     </row>
     <row r="17" spans="1:14" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="G17" s="3">
-        <v>1298.741047992</v>
+        <v>1602.91580999</v>
       </c>
       <c r="H17" s="3">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -8356,10 +9241,10 @@
     </row>
     <row r="18" spans="1:14" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -8368,7 +9253,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -8378,10 +9263,10 @@
     </row>
     <row r="19" spans="1:14" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -8390,7 +9275,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -8400,19 +9285,29 @@
     </row>
     <row r="20" spans="1:14" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+        <v>167</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="3">
+        <v>322.165761998</v>
+      </c>
+      <c r="H20" s="3">
+        <v>-2</v>
+      </c>
       <c r="I20" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -8422,19 +9317,29 @@
     </row>
     <row r="21" spans="1:14" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+        <v>171</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G21" s="3">
+        <v>480.1072859940001</v>
+      </c>
+      <c r="H21" s="3">
+        <v>-4</v>
+      </c>
       <c r="I21" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -8444,10 +9349,10 @@
     </row>
     <row r="22" spans="1:14" ht="15.01" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -8456,7 +9361,7 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -8532,10 +9437,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>84</v>
@@ -8558,7 +9463,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
@@ -8568,7 +9473,7 @@
         <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -8578,17 +9483,17 @@
     </row>
     <row r="3" spans="1:10" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -8598,17 +9503,17 @@
     </row>
     <row r="4" spans="1:10" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -8618,17 +9523,17 @@
     </row>
     <row r="5" spans="1:10" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -8638,17 +9543,17 @@
     </row>
     <row r="6" spans="1:10" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -8658,17 +9563,17 @@
     </row>
     <row r="7" spans="1:10" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -8678,17 +9583,17 @@
     </row>
     <row r="8" spans="1:10" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -8698,17 +9603,17 @@
     </row>
     <row r="9" spans="1:10" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -8718,17 +9623,17 @@
     </row>
     <row r="10" spans="1:10" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -8738,17 +9643,17 @@
     </row>
     <row r="11" spans="1:10" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -8758,17 +9663,17 @@
     </row>
     <row r="12" spans="1:10" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -8778,17 +9683,17 @@
     </row>
     <row r="13" spans="1:10" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -8798,17 +9703,17 @@
     </row>
     <row r="14" spans="1:10" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -8818,17 +9723,17 @@
     </row>
     <row r="15" spans="1:10" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -8838,17 +9743,17 @@
     </row>
     <row r="16" spans="1:10" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -8858,17 +9763,17 @@
     </row>
     <row r="17" spans="1:10" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -8878,17 +9783,17 @@
     </row>
     <row r="18" spans="1:10" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -8898,17 +9803,17 @@
     </row>
     <row r="19" spans="1:10" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -8918,17 +9823,17 @@
     </row>
     <row r="20" spans="1:10" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -8938,17 +9843,17 @@
     </row>
     <row r="21" spans="1:10" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -9043,11 +9948,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>92</v>
@@ -9057,7 +9962,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -9067,11 +9972,11 @@
     </row>
     <row r="3" spans="1:12" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>92</v>
@@ -9081,7 +9986,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -9091,11 +9996,11 @@
     </row>
     <row r="4" spans="1:12" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>179</v>
+        <v>201</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>92</v>
@@ -9105,7 +10010,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -9115,11 +10020,11 @@
     </row>
     <row r="5" spans="1:12" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>180</v>
+        <v>202</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>92</v>
@@ -9129,7 +10034,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -9139,11 +10044,11 @@
     </row>
     <row r="6" spans="1:12" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>92</v>
@@ -9153,7 +10058,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -9163,11 +10068,11 @@
     </row>
     <row r="7" spans="1:12" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>92</v>
@@ -9177,7 +10082,7 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -9187,11 +10092,11 @@
     </row>
     <row r="8" spans="1:12" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>92</v>
@@ -9201,7 +10106,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -9211,11 +10116,11 @@
     </row>
     <row r="9" spans="1:12" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>92</v>
@@ -9225,7 +10130,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -9235,11 +10140,11 @@
     </row>
     <row r="10" spans="1:12" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>185</v>
+        <v>207</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>92</v>
@@ -9249,7 +10154,7 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -9259,11 +10164,11 @@
     </row>
     <row r="11" spans="1:12" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>92</v>
@@ -9273,7 +10178,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -9283,11 +10188,11 @@
     </row>
     <row r="12" spans="1:12" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>92</v>
@@ -9297,7 +10202,7 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -9307,11 +10212,11 @@
     </row>
     <row r="13" spans="1:12" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>92</v>
@@ -9321,7 +10226,7 @@
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -9331,11 +10236,11 @@
     </row>
     <row r="14" spans="1:12" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>92</v>
@@ -9345,7 +10250,7 @@
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -9355,11 +10260,11 @@
     </row>
     <row r="15" spans="1:12" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>92</v>
@@ -9369,7 +10274,7 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -9379,11 +10284,11 @@
     </row>
     <row r="16" spans="1:12" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>92</v>
@@ -9393,7 +10298,7 @@
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -9403,11 +10308,11 @@
     </row>
     <row r="17" spans="1:12" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>92</v>
@@ -9417,7 +10322,7 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -9427,11 +10332,11 @@
     </row>
     <row r="18" spans="1:12" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>92</v>
@@ -9441,7 +10346,7 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -9451,11 +10356,11 @@
     </row>
     <row r="19" spans="1:12" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>92</v>
@@ -9465,7 +10370,7 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -9475,11 +10380,11 @@
     </row>
     <row r="20" spans="1:12" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>92</v>
@@ -9489,7 +10394,7 @@
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -9499,11 +10404,11 @@
     </row>
     <row r="21" spans="1:12" ht="15.01" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>92</v>
@@ -9513,7 +10418,7 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>

</xml_diff>

<commit_message>
simple rna model ntp synthesis
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model.xlsx
+++ b/rand_wc_model_gen/model_gen/model.xlsx
@@ -45,9 +45,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Observables!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'Observation sets'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Observations!$A$2:$W$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$20</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Parameters!$A$1:$K$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Rate laws'!$A$1:$L$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$2:$N$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">References!$A$1:$R$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Species types'!$A$2:$N$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Species!$A$1:$J$21</definedName>
@@ -4215,7 +4215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="358">
   <si>
     <t>'Model'!A1</t>
   </si>
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-14 13:49:08</t>
+    <t>2019-08-14 15:07:43</t>
   </si>
   <si>
     <t>Updated</t>
@@ -4934,6 +4934,42 @@
     <t>[c]: (4) h2o + rna_3 ==&gt; amp + (2) cmp + gmp + (4) h + ump</t>
   </si>
   <si>
+    <t>syn_atp</t>
+  </si>
+  <si>
+    <t>synthesis ATP</t>
+  </si>
+  <si>
+    <t>[c]: amp + h + ppi ==&gt; atp + h2o</t>
+  </si>
+  <si>
+    <t>syn_ctp</t>
+  </si>
+  <si>
+    <t>synthesis CTP</t>
+  </si>
+  <si>
+    <t>[c]: cmp + h + ppi ==&gt; ctp + h2o</t>
+  </si>
+  <si>
+    <t>syn_gtp</t>
+  </si>
+  <si>
+    <t>synthesis GTP</t>
+  </si>
+  <si>
+    <t>[c]: gmp + h + ppi ==&gt; gtp + h2o</t>
+  </si>
+  <si>
+    <t>syn_utp</t>
+  </si>
+  <si>
+    <t>synthesis UTP</t>
+  </si>
+  <si>
+    <t>[c]: h + ppi + ump ==&gt; h2o + utp</t>
+  </si>
+  <si>
     <t>transcription_rna_1</t>
   </si>
   <si>
@@ -4988,6 +5024,30 @@
     <t>k_deg_rna_3 * rna_3[c] / (km_deg_rna_3 * Avogadro * volume_c + rna_3[c])</t>
   </si>
   <si>
+    <t>syn_atp-forward</t>
+  </si>
+  <si>
+    <t>k_syn_atp * (amp[c] / (km_syn_atp_amp * Avogadro * volume_c + amp[c])) * (ppi[c] / (km_syn_ntp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_ctp-forward</t>
+  </si>
+  <si>
+    <t>k_syn_ctp * (cmp[c] / (km_syn_ctp_cmp * Avogadro * volume_c + cmp[c])) * (ppi[c] / (km_syn_ntp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_gtp-forward</t>
+  </si>
+  <si>
+    <t>k_syn_gtp * (gmp[c] / (km_syn_gtp_gmp * Avogadro * volume_c + gmp[c])) * (ppi[c] / (km_syn_ntp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
+    <t>syn_utp-forward</t>
+  </si>
+  <si>
+    <t>k_syn_utp * (ump[c] / (km_syn_utp_ump * Avogadro * volume_c + ump[c])) * (ppi[c] / (km_syn_ntp_ppi * Avogadro * volume_c + ppi[c]))</t>
+  </si>
+  <si>
     <t>transcription_rna_1-forward</t>
   </si>
   <si>
@@ -5054,6 +5114,18 @@
     <t>k_deg_rna_3</t>
   </si>
   <si>
+    <t>k_syn_atp</t>
+  </si>
+  <si>
+    <t>k_syn_ctp</t>
+  </si>
+  <si>
+    <t>k_syn_gtp</t>
+  </si>
+  <si>
+    <t>k_syn_utp</t>
+  </si>
+  <si>
     <t>k_trans_rna_1</t>
   </si>
   <si>
@@ -5085,6 +5157,21 @@
   </si>
   <si>
     <t>km_gtp_trans</t>
+  </si>
+  <si>
+    <t>km_syn_atp_amp</t>
+  </si>
+  <si>
+    <t>km_syn_ctp_cmp</t>
+  </si>
+  <si>
+    <t>km_syn_gtp_gmp</t>
+  </si>
+  <si>
+    <t>km_syn_ntp_ppi</t>
+  </si>
+  <si>
+    <t>km_syn_utp_ump</t>
   </si>
   <si>
     <t>km_utp_trans</t>
@@ -5703,7 +5790,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.01" customHeight="1">
@@ -5712,7 +5799,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.01" customHeight="1">
@@ -5748,7 +5835,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.01" customHeight="1">
@@ -6007,7 +6094,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -6254,47 +6341,159 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
+    <row r="9" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" ht="15.01" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A2:N8"/>
+  <autoFilter ref="A2:N12"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A8">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A3:A12">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B8">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B3:B12">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C8">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." sqref="C3:C12">
       <formula1>'Submodels'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D8"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E8">
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" sqref="D3:D12"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E12">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F8">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="F3:F12">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G8">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." sqref="G3:G12">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H8">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="H3:H12">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I8">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." sqref="I3:I12">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J8"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K8"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L8"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M8">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="J3:J12"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="K3:K12"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="L3:L12"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="M3:M12">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N8"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="N3:N12"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6303,7 +6502,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6324,10 +6523,10 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>103</v>
@@ -6356,18 +6555,18 @@
     </row>
     <row r="2" spans="1:12" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>229</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>232</v>
@@ -6380,18 +6579,18 @@
     </row>
     <row r="3" spans="1:12" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
         <v>233</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>232</v>
@@ -6404,18 +6603,18 @@
     </row>
     <row r="4" spans="1:12" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
         <v>236</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>232</v>
@@ -6428,18 +6627,18 @@
     </row>
     <row r="5" spans="1:12" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
         <v>239</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>232</v>
@@ -6452,18 +6651,18 @@
     </row>
     <row r="6" spans="1:12" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>242</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>232</v>
@@ -6476,18 +6675,18 @@
     </row>
     <row r="7" spans="1:12" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>245</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>232</v>
@@ -6498,36 +6697,132 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
+    <row r="8" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.01" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:L7"/>
+  <autoFilter ref="A1:L11"/>
   <dataValidations count="12">
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A7">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." sqref="A2:A11">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B7">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B11">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C7">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." sqref="C2:C11">
       <formula1>'Reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D7">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." sqref="D2:D11">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E7">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." sqref="E2:E11">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F7"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G7">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." sqref="F2:F11"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." sqref="G2:G11">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H7"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I7"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J7"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K7">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="H2:H11"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="I2:I11"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="J2:J11"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="K2:K11">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L7"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="L2:L11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6566,10 +6861,10 @@
         <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>62</v>
@@ -6652,7 +6947,7 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>62</v>
@@ -6726,7 +7021,7 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>32</v>
@@ -6791,7 +7086,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6818,7 +7113,7 @@
         <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>84</v>
@@ -6841,7 +7136,7 @@
     </row>
     <row r="2" spans="1:11" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6850,7 +7145,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -6860,7 +7155,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6888,7 +7183,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6898,7 +7193,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.01" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6917,7 +7212,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.01" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6936,7 +7231,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.01" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6955,11 +7250,11 @@
     </row>
     <row r="8" spans="1:11" ht="15.01" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D8" s="3">
         <v>0.003850817669777474</v>
@@ -6976,11 +7271,11 @@
     </row>
     <row r="9" spans="1:11" ht="15.01" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D9" s="3">
         <v>0.003850817669777474</v>
@@ -6997,11 +7292,11 @@
     </row>
     <row r="10" spans="1:11" ht="15.01" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D10" s="3">
         <v>0.003850817669777474</v>
@@ -7018,11 +7313,11 @@
     </row>
     <row r="11" spans="1:11" ht="15.01" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D11" s="3">
         <v>0.03080654135821979</v>
@@ -7039,11 +7334,11 @@
     </row>
     <row r="12" spans="1:11" ht="15.01" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D12" s="3">
         <v>0.03080654135821979</v>
@@ -7060,11 +7355,11 @@
     </row>
     <row r="13" spans="1:11" ht="15.01" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="D13" s="3">
         <v>0.03080654135821979</v>
@@ -7081,18 +7376,18 @@
     </row>
     <row r="14" spans="1:11" ht="15.01" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="D14" s="3">
-        <v>0.005</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -7102,18 +7397,18 @@
     </row>
     <row r="15" spans="1:11" ht="15.01" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="D15" s="3">
-        <v>0.005</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -7123,18 +7418,18 @@
     </row>
     <row r="16" spans="1:11" ht="15.01" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="D16" s="3">
-        <v>1</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -7144,18 +7439,18 @@
     </row>
     <row r="17" spans="1:11" ht="15.01" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>0.03080654135821979</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -7165,18 +7460,18 @@
     </row>
     <row r="18" spans="1:11" ht="15.01" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="D18" s="3">
-        <v>1</v>
+        <v>0.005</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -7186,18 +7481,18 @@
     </row>
     <row r="19" spans="1:11" ht="15.01" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="D19" s="3">
         <v>0.005</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -7207,18 +7502,18 @@
     </row>
     <row r="20" spans="1:11" ht="15.01" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="D20" s="3">
-        <v>0.005</v>
+        <v>3.321078080854328e-08</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -7226,35 +7521,224 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
+    <row r="21" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3.321078080854328e-08</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3.321078080854328e-08</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D24" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D25" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D26" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D28" s="3">
+        <v>5e-05</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.01" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.005</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:K20"/>
+  <autoFilter ref="A1:K29"/>
   <dataValidations count="11">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A20">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." sqref="A2:A29">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B20">
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B2:B29">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C20">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." sqref="C2:C29">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D20">
+    <dataValidation type="decimal" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." sqref="D2:D29">
       <formula1>-1e+100</formula1>
       <formula2>1e+100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E20">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." sqref="E2:E29">
       <formula1>-1e-100</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F20"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G20"/>
-    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H20"/>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I20"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J20">
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." sqref="F2:F29"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" sqref="G2:G29"/>
+    <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" sqref="H2:H29"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." sqref="I2:I29"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." sqref="J2:J29">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K20"/>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="K2:K29"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7356,10 +7840,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>291</v>
+        <v>320</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>291</v>
+        <v>320</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>28</v>
@@ -7382,16 +7866,16 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
@@ -7408,7 +7892,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7420,7 +7904,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>68</v>
@@ -7432,19 +7916,19 @@
         <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>296</v>
+        <v>325</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>298</v>
+        <v>327</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>299</v>
+        <v>328</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>51</v>
@@ -7774,10 +8258,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5" t="s">
-        <v>300</v>
+        <v>329</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>300</v>
+        <v>329</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -7797,7 +8281,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
@@ -7827,7 +8311,7 @@
         <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>301</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -7900,46 +8384,46 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>302</v>
+        <v>331</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>303</v>
+        <v>332</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>304</v>
+        <v>333</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>306</v>
+        <v>335</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>307</v>
+        <v>336</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>308</v>
+        <v>337</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>309</v>
+        <v>338</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>311</v>
+        <v>340</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>62</v>
@@ -8034,28 +8518,28 @@
         <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>302</v>
+        <v>331</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>318</v>
+        <v>347</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>319</v>
+        <v>348</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>320</v>
+        <v>349</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -8138,25 +8622,25 @@
         <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>323</v>
+        <v>352</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>326</v>
+        <v>355</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>327</v>
+        <v>356</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>328</v>
+        <v>357</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>62</v>
@@ -8177,7 +8661,7 @@
         <v>47</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>301</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run simulation and plot rna results
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model.xlsx
+++ b/rand_wc_model_gen/model_gen/model.xlsx
@@ -4412,7 +4412,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>2019-08-16 18:41:28</t>
+    <t>2019-08-19 12:43:06</t>
   </si>
   <si>
     <t>Updated</t>
@@ -7323,7 +7323,7 @@
         <v>296</v>
       </c>
       <c r="D11" s="3">
-        <v>0.03080654135821979</v>
+        <v>0.003080654135821979</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
@@ -7344,7 +7344,7 @@
         <v>296</v>
       </c>
       <c r="D12" s="3">
-        <v>0.03080654135821979</v>
+        <v>0.003080654135821979</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
@@ -7365,7 +7365,7 @@
         <v>296</v>
       </c>
       <c r="D13" s="3">
-        <v>0.03080654135821979</v>
+        <v>0.003080654135821979</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
@@ -7386,7 +7386,7 @@
         <v>296</v>
       </c>
       <c r="D14" s="3">
-        <v>0.03080654135821979</v>
+        <v>0.003080654135821979</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
@@ -7470,7 +7470,7 @@
         <v>308</v>
       </c>
       <c r="D18" s="3">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
@@ -7491,7 +7491,7 @@
         <v>308</v>
       </c>
       <c r="D19" s="3">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -7575,7 +7575,7 @@
         <v>308</v>
       </c>
       <c r="D23" s="3">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
@@ -7596,7 +7596,7 @@
         <v>308</v>
       </c>
       <c r="D24" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
@@ -7617,7 +7617,7 @@
         <v>308</v>
       </c>
       <c r="D25" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
@@ -7638,7 +7638,7 @@
         <v>308</v>
       </c>
       <c r="D26" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -7680,7 +7680,7 @@
         <v>308</v>
       </c>
       <c r="D28" s="3">
-        <v>5e-05</v>
+        <v>0.001</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
@@ -7701,7 +7701,7 @@
         <v>308</v>
       </c>
       <c r="D29" s="3">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
@@ -10445,7 +10445,7 @@
         <v>92</v>
       </c>
       <c r="E2" s="3">
-        <v>1505.53521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
@@ -10469,7 +10469,7 @@
         <v>92</v>
       </c>
       <c r="E3" s="3">
-        <v>150553.521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
@@ -10517,7 +10517,7 @@
         <v>92</v>
       </c>
       <c r="E5" s="3">
-        <v>1505.53521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
@@ -10541,7 +10541,7 @@
         <v>92</v>
       </c>
       <c r="E6" s="3">
-        <v>150553.521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
@@ -10589,7 +10589,7 @@
         <v>92</v>
       </c>
       <c r="E8" s="3">
-        <v>1505.53521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
@@ -10613,7 +10613,7 @@
         <v>92</v>
       </c>
       <c r="E9" s="3">
-        <v>150553.521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -10661,7 +10661,7 @@
         <v>92</v>
       </c>
       <c r="E11" s="3">
-        <v>15055.3521425</v>
+        <v>1656088735.675</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
@@ -10853,7 +10853,7 @@
         <v>92</v>
       </c>
       <c r="E19" s="3">
-        <v>1505.53521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
@@ -10877,7 +10877,7 @@
         <v>92</v>
       </c>
       <c r="E20" s="3">
-        <v>150553.521425</v>
+        <v>30110.704285</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">

</xml_diff>

<commit_message>
updating for obj_tables, wc_kb, and wc_lang
</commit_message>
<xml_diff>
--- a/rand_wc_model_gen/model_gen/model.xlsx
+++ b/rand_wc_model_gen/model_gen/model.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13965" windowWidth="28695"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28695" windowHeight="13965" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!_Table of contents" sheetId="1" state="visible" r:id="rId1"/>
@@ -32,27 +32,27 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="!!Changes" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'!!_Table of contents'!$A$1:$C$24</definedName>
-    <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'!!Submodels'!$A$1:$H$2</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">'!!Compartments'!$A$2:$U$3</definedName>
-    <definedName hidden="1" localSheetId="6" name="_xlnm._FilterDatabase">'!!Species types'!$A$2:$N$22</definedName>
-    <definedName hidden="1" localSheetId="7" name="_xlnm._FilterDatabase">'!!Species'!$A$1:$J$21</definedName>
-    <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">'!!Init species concentrations'!$A$1:$L$21</definedName>
-    <definedName hidden="1" localSheetId="9" name="_xlnm._FilterDatabase">'!!Observables'!$A$1:$I$1</definedName>
-    <definedName hidden="1" localSheetId="10" name="_xlnm._FilterDatabase">'!!Functions'!$A$1:$I$2</definedName>
-    <definedName hidden="1" localSheetId="11" name="_xlnm._FilterDatabase">'!!Reactions'!$A$2:$N$12</definedName>
-    <definedName hidden="1" localSheetId="12" name="_xlnm._FilterDatabase">'!!Rate laws'!$A$1:$L$11</definedName>
-    <definedName hidden="1" localSheetId="13" name="_xlnm._FilterDatabase">'!!dFBA objectives'!$A$1:$L$1</definedName>
-    <definedName hidden="1" localSheetId="14" name="_xlnm._FilterDatabase">'!!dFBA objective reactions'!$A$1:$J$1</definedName>
-    <definedName hidden="1" localSheetId="15" name="_xlnm._FilterDatabase">'!!dFBA objective species'!$A$1:$K$1</definedName>
-    <definedName hidden="1" localSheetId="16" name="_xlnm._FilterDatabase">'!!Parameters'!$A$1:$K$29</definedName>
-    <definedName hidden="1" localSheetId="17" name="_xlnm._FilterDatabase">'!!Stop conditions'!$A$1:$I$1</definedName>
-    <definedName hidden="1" localSheetId="18" name="_xlnm._FilterDatabase">'!!Observations'!$A$2:$W$2</definedName>
-    <definedName hidden="1" localSheetId="19" name="_xlnm._FilterDatabase">'!!Observation sets'!$A$1:$F$1</definedName>
-    <definedName hidden="1" localSheetId="20" name="_xlnm._FilterDatabase">'!!Conclusions'!$A$2:$N$2</definedName>
-    <definedName hidden="1" localSheetId="21" name="_xlnm._FilterDatabase">'!!References'!$A$1:$R$1</definedName>
-    <definedName hidden="1" localSheetId="22" name="_xlnm._FilterDatabase">'!!Authors'!$A$1:$L$1</definedName>
-    <definedName hidden="1" localSheetId="23" name="_xlnm._FilterDatabase">'!!Changes'!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$1:$C$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'!!Submodels'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$U$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$N$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'!!Species'!$A$1:$J$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'!!Init species concentrations'!$A$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'!!Observables'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'!!Functions'!$A$1:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$N$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Rate laws'!$A$1:$L$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'!!dFBA objectives'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'!!dFBA objective reactions'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'!!dFBA objective species'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$K$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'!!Stop conditions'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'!!Observations'!$A$2:$W$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">'!!Observation sets'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">'!!Conclusions'!$A$2:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'!!Authors'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">'!!Changes'!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
@@ -61,9 +61,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="164"/>
-    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="165"/>
-    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="166"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -558,220 +558,220 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="8" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="34" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="22" numFmtId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="7" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="20" numFmtId="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="18" numFmtId="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="35" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="16" numFmtId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="5" fillId="13" fontId="15" numFmtId="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="10" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="29" fontId="21" numFmtId="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="13" fontId="19" numFmtId="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="17" numFmtId="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="11" numFmtId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="165">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="5" numFmtId="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="13" numFmtId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="166">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="6" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="8" numFmtId="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="1"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="2"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="3"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="4"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="5"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="6"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="7"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="8"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="9"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="10"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="11"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="12"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="13"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="14"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="16"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="17"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="18"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="19"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="20"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="21"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="22"/>
-    <cellStyle builtinId="27" name="Bad" xfId="23"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="24"/>
-    <cellStyle builtinId="25" name="Total" xfId="25"/>
-    <cellStyle builtinId="21" name="Output" xfId="26"/>
-    <cellStyle builtinId="4" name="Currency" xfId="27"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="28"/>
-    <cellStyle builtinId="10" name="Note" xfId="29"/>
-    <cellStyle builtinId="20" name="Input" xfId="30"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="31"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="32"/>
-    <cellStyle builtinId="26" name="Good" xfId="33"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="34"/>
-    <cellStyle builtinId="53" name="CExplanatory Text" xfId="35"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="36"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="37"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="38"/>
-    <cellStyle builtinId="15" name="Title" xfId="39"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="40"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="41"/>
-    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="42"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="43"/>
-    <cellStyle builtinId="3" name="Comma" xfId="44"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="45"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="46"/>
-    <cellStyle builtinId="5" name="Percent" xfId="47"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="48"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -781,7 +781,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -789,48 +789,48 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A4" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A5" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <t>Enter a valid URL
 Enter a string.
 Value must be less than or equal to 65535 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A6" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A7" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A8" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A9" shapeId="0">
+    <comment ref="A9" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A10" shapeId="0">
+    <comment ref="A10" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -838,18 +838,18 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A11" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A12" shapeId="0">
+    <comment ref="A12" authorId="0" shapeId="0">
       <text>
         <t>Enter a date and time.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A13" shapeId="0">
+    <comment ref="A13" authorId="0" shapeId="0">
       <text>
         <t>Enter a date and time.</t>
       </text>
@@ -864,7 +864,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -872,24 +872,24 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a expression of Compartments, Functions, Observables, Parameters and Species.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Enter a unit or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -897,7 +897,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -906,18 +906,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -932,7 +932,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -940,18 +940,18 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Submodels:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <t>Enter a reaction string using species from "Species:A".
 Examples:
@@ -960,36 +960,36 @@
 * (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E3" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <t>Enter a Boolean value
 Select "True" or "False".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F3" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "1 / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H3" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I3" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "molar / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J3" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -997,7 +997,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K3" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1006,18 +1006,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L3" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M3" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N3" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1032,46 +1032,46 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Reactions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Select one of "backward", "forward".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "Michaelis_Menten_rate_law", "hill_rate_law", "mass_action_rate_law", "modular_rate_law" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a expression of Compartments, Functions, Observables, Parameters and Species.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "1 / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1079,7 +1079,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1088,18 +1088,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1114,48 +1114,48 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Submodels:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a expression of dFBA objective reactions and Reactions.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "dimensionless" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "1 / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1163,7 +1163,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1172,18 +1172,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1198,7 +1198,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1206,30 +1206,30 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Submodels:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "1 / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "liter", "gDCW" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1237,7 +1237,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1246,18 +1246,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1272,41 +1272,41 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "dFBA objective reactions:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Species:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "molar / second", "mole / gDCW / second" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1314,7 +1314,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1323,18 +1323,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1349,7 +1349,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1357,35 +1357,35 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "kinetic_constant", "K_i", "K_m", "k_cat", "v_max" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Enter a unit or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1393,7 +1393,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1402,18 +1402,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1428,7 +1428,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1436,24 +1436,24 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a expression of Compartments, Functions, Observables, Parameters and Species.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "dimensionless" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1461,7 +1461,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1470,18 +1470,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1496,7 +1496,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1504,118 +1504,118 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E3" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Enter a unit or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F3" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "computational_observation", "experimental_observation", "theoretical_observation" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H3" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I3" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J3" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "degC" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K3" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L3" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "dimensionless" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M3" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N3" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="O3" shapeId="0">
+    <comment ref="O3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="P3" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Q3" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="R3" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="S3" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="T3" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="U3" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1623,13 +1623,13 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="V3" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="W3" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1644,7 +1644,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1652,18 +1652,18 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Observations:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1671,13 +1671,13 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1692,24 +1692,24 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A4" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <t>Select one of "domain", "kingdom", "phylum", "classis", "order", "family", "tribe", "genus", "species", "variety".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A5" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1717,13 +1717,13 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A6" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A7" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -1738,7 +1738,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1746,48 +1746,48 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E3" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Enter a unit or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F3" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "approximation", "assumption", "computation", "decision" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H3" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I3" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1795,7 +1795,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J3" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -1804,23 +1804,23 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K3" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L3" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M3" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Authors:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N3" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <t>Enter a date and time.</t>
       </text>
@@ -1835,7 +1835,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1843,96 +1843,96 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter an integer.
 Value must be positive.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "article", "book", "preprint", "proceedings", "supplementary_material", "thesis", "website" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M2" shapeId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N2" shapeId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="O2" shapeId="0">
+    <comment ref="O2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="P2" shapeId="0">
+    <comment ref="P2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Q2" shapeId="0">
+    <comment ref="Q2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -1940,7 +1940,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="R2" shapeId="0">
+    <comment ref="R2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
@@ -1956,7 +1956,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -1964,63 +1964,63 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be between 1 and 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be between 1 and 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be between 1 and 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a valid email address
 Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a valid URL
 Enter a string.
 Value must be less than or equal to 65535 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2028,7 +2028,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
@@ -2044,7 +2044,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -2052,56 +2052,56 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be between 1 and 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "copy", "deletion_change_provenance", "insertion", "merge", "move", "revert", "update" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Submodels:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "data_target_provenance", "encoding_target_provenance", "metadata_target_provenance", "model_target_provenance", "model_dynamics_target_provenance", "model_initial_conditions_target_provenance" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "add_metadata_reason_provenance", "implementation_error_reason_provenance", "incorrect_interpretation_reason_provenance", "migrate_version_reason_provenance", "new_goal_reason_provenance", "new_knowledge_reason_provenance" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "correct_intention_provenance", "elaborate_intention_provenance", "expand_intention_provenance", "simplify_intention_provenance" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2109,7 +2109,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2118,28 +2118,28 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M2" shapeId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N2" shapeId="0">
+    <comment ref="N2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="O2" shapeId="0">
+    <comment ref="O2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="P2" shapeId="0">
+    <comment ref="P2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Authors:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Q2" shapeId="0">
+    <comment ref="Q2" authorId="0" shapeId="0">
       <text>
         <t>Enter a date and time.</t>
       </text>
@@ -2154,30 +2154,30 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A4" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A5" shapeId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "degC" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A6" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2185,13 +2185,13 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A7" shapeId="0">
+    <comment ref="A7" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A8" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2206,7 +2206,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -2214,18 +2214,18 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "dynamic_flux_balance_analysis", "ordinary_differential_equations", "stochastic_simulation_algorithm".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2233,7 +2233,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2242,18 +2242,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2268,7 +2268,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -2276,89 +2276,89 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "cellular_compartment", "extracellular_compartment" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "fluid_compartment", "membrane_compartment" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E3" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "3D_compartment" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F3" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Compartments:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "gram" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H3" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "Dirichlet_distribution", "Gumbel_distribution", "Laplace_distribution", "Pareto_distribution", "Poisson_distribution", "Rayleigh_distribution", "Vonmises_distribution", "Wald_distribution", "Weibull_distribution", "Zipf_distribution", "beta_distribution", "binomial_distribution", "chi_square_distribution", "exponential_distribution", "f_distribution", "gamma_distribution", "geometric_distribution", "hypergeometric_distribution", "log_normal_distribution", "log_series_distribution", "logisitic_distribution", "multinomial_distribution", "multivariate_normal_distribution", "negative_binomial_distribution", "noncentral-chi_square_distribution", "noncentral-f_distribution", "normal_distribution", "power_distribution", "standard-Cauchy_distribution", "standard-exponential_distribution", "standard-gamma_distribution", "standard-normal_distribution", "standard-t_distribution", "triangular_distribution", "uniform_distribution" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I3" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J3" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K3" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "liter" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L3" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Parameters:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M3" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "Dirichlet_distribution", "Gumbel_distribution", "Laplace_distribution", "Pareto_distribution", "Poisson_distribution", "Rayleigh_distribution", "Vonmises_distribution", "Wald_distribution", "Weibull_distribution", "Zipf_distribution", "beta_distribution", "binomial_distribution", "chi_square_distribution", "exponential_distribution", "f_distribution", "gamma_distribution", "geometric_distribution", "hypergeometric_distribution", "log_normal_distribution", "log_series_distribution", "logisitic_distribution", "multinomial_distribution", "multivariate_normal_distribution", "negative_binomial_distribution", "noncentral-chi_square_distribution", "noncentral-f_distribution", "normal_distribution", "power_distribution", "standard-Cauchy_distribution", "standard-exponential_distribution", "standard-gamma_distribution", "standard-normal_distribution", "standard-t_distribution", "triangular_distribution", "uniform_distribution" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N3" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="O3" shapeId="0">
+    <comment ref="O3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="P3" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "dimensionless" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="Q3" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2366,7 +2366,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="R3" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2375,18 +2375,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="S3" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="T3" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="U3" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2401,7 +2401,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A3" shapeId="0">
+    <comment ref="A3" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -2409,51 +2409,51 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B3" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C3" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <t>Select one of "smiles", "bpforms" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E3" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <t>Select one of "dna", "rna", "protein", "canonical_dna", "canonical_rna", "canonical_protein" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F3" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <t>An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')
 Enter an empirical formula (e.g. "H2O").</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G3" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H3" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <t>Enter an integer.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I3" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "DNA", "RNA", "complex", "metabolite", "protein", "pseudo_species", "asRNA", "intergenic", "mRNA", "mixed", "ncRNA", "rRNA", "sRNA", "tRNA", "TRNASynthClassIIComplex", "fattyAcylAcpComplex", "Ion", "aminoAcid", "carbohydrateSugar", "carbohydrateSugarPhosphate", "carboxyAcid", "dipeptide", "modifiedNucleobase", "nucleobase", "reactiveOxygenSpecies", "ribonucleotideBiphosphate", "ribonucleotideMonophosphate", "ribonucleotideTriphosphate", "vitamin", "TRNASynthClassI", "TRNASynthClassIB", "TRNASynthClassII" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J3" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2461,7 +2461,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K3" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2470,18 +2470,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L3" shapeId="0">
+    <comment ref="L3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="M3" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="N3" shapeId="0">
+    <comment ref="N3" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2496,36 +2496,36 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Species types:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Compartments:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "molecule" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2533,7 +2533,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2542,18 +2542,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2568,48 +2568,48 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Select a value from "Species:A".</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of WC ontology terms "Dirichlet_distribution", "Gumbel_distribution", "Laplace_distribution", "Pareto_distribution", "Poisson_distribution", "Rayleigh_distribution", "Vonmises_distribution", "Wald_distribution", "Weibull_distribution", "Zipf_distribution", "beta_distribution", "binomial_distribution", "chi_square_distribution", "exponential_distribution", "f_distribution", "gamma_distribution", "geometric_distribution", "hypergeometric_distribution", "log_normal_distribution", "log_series_distribution", "logisitic_distribution", "multinomial_distribution", "multivariate_normal_distribution", "negative_binomial_distribution", "noncentral-chi_square_distribution", "noncentral-f_distribution", "normal_distribution", "power_distribution", "standard-Cauchy_distribution", "standard-exponential_distribution", "standard-gamma_distribution", "standard-normal_distribution", "standard-t_distribution", "triangular_distribution", "uniform_distribution" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a float or blank.
 Value must be greater than or equal to 0.0.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "molecule", "molar", "millimolar", "micromolar", "nanomolar", "picomolar", "femtomolar", "attomolar" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2617,7 +2617,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2626,18 +2626,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K2" shapeId="0">
+    <comment ref="K2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L2" shapeId="0">
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -2652,7 +2652,7 @@
     <author>None</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A2" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <t>Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number
 Enter a string.
@@ -2660,24 +2660,24 @@
 Value must be unique.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 255 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="C2" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <t>Enter a linear expression of Observables and Species.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <t>Units (e.g. 'second', 'meter', or 'gram')
 Select one unit of "molecule" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E2" shapeId="0">
+    <comment ref="E2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of identifiers in external namespaces.
 Examples:
@@ -2685,7 +2685,7 @@
 * chebi: CHEBI:15377, kegg.compound: C00001</t>
       </text>
     </comment>
-    <comment authorId="0" ref="F2" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <t>Enter a list of observations from "Observations:A".
 Examples:
@@ -2694,18 +2694,18 @@
 * Obs4(+, q=30)</t>
       </text>
     </comment>
-    <comment authorId="0" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "Conclusions:A" or blank.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="H2" shapeId="0">
+    <comment ref="H2" authorId="0" shapeId="0">
       <text>
         <t>Enter a string.
 Value must be less than or equal to 4294967295 characters.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <t>Enter a comma-separated list of values from "References:A" or blank.</t>
       </text>
@@ -3005,28 +3005,28 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="3" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="4" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="3"/>
+    <col hidden="1" width="9" customWidth="1" min="4" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
+          <t>!!!ObjTables objTablesVersion='0.0.8'</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Schema' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Schema' objTablesVersion='0.0.8' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -3303,31 +3303,31 @@
   </sheetData>
   <autoFilter ref="A1:C24"/>
   <hyperlinks>
-    <hyperlink display="Model" location="'Model'!A1" ref="A2" tooltip="Click to view model"/>
-    <hyperlink display="Taxon" location="'Taxon'!A1" ref="A3" tooltip="Click to view taxon"/>
-    <hyperlink display="Environment" location="'Environment'!A1" ref="A4" tooltip="Click to view environment"/>
-    <hyperlink display="Submodels" location="'Submodels'!A1" ref="A5" tooltip="Click to view submodels"/>
-    <hyperlink display="Compartments" location="'Compartments'!A1" ref="A6" tooltip="Click to view compartments"/>
-    <hyperlink display="Species types" location="'Species types'!A1" ref="A7" tooltip="Click to view species types"/>
-    <hyperlink display="Species" location="'Species'!A1" ref="A8" tooltip="Click to view species"/>
-    <hyperlink display="Initial species concentrations" location="'Initial species concentrations'!A1" ref="A9" tooltip="Click to view initial species concentrations"/>
-    <hyperlink display="Observables" location="'Observables'!A1" ref="A10" tooltip="Click to view observables"/>
-    <hyperlink display="Functions" location="'Functions'!A1" ref="A11" tooltip="Click to view functions"/>
-    <hyperlink display="Reactions" location="'Reactions'!A1" ref="A12" tooltip="Click to view reactions"/>
-    <hyperlink display="Rate laws" location="'Rate laws'!A1" ref="A13" tooltip="Click to view rate laws"/>
-    <hyperlink display="dFBA objectives" location="'dFBA objectives'!A1" ref="A14" tooltip="Click to view dfba objectives"/>
-    <hyperlink display="dFBA objective reactions" location="'dFBA objective reactions'!A1" ref="A15" tooltip="Click to view dfba objective reactions"/>
-    <hyperlink display="dFBA objective species" location="'dFBA objective species'!A1" ref="A16" tooltip="Click to view dfba objective species"/>
-    <hyperlink display="Parameters" location="'Parameters'!A1" ref="A17" tooltip="Click to view parameters"/>
-    <hyperlink display="Stop conditions" location="'Stop conditions'!A1" ref="A18" tooltip="Click to view stop conditions"/>
-    <hyperlink display="Observations" location="'Observations'!A1" ref="A19" tooltip="Click to view observations"/>
-    <hyperlink display="Observation sets" location="'Observation sets'!A1" ref="A20" tooltip="Click to view observation sets"/>
-    <hyperlink display="Conclusions" location="'Conclusions'!A1" ref="A21" tooltip="Click to view conclusions"/>
-    <hyperlink display="References" location="'References'!A1" ref="A22" tooltip="Click to view references"/>
-    <hyperlink display="Authors" location="'Authors'!A1" ref="A23" tooltip="Click to view authors"/>
-    <hyperlink display="Changes" location="'Changes'!A1" ref="A24" tooltip="Click to view changes"/>
+    <hyperlink ref="A2" location="'Model'!A1" tooltip="Click to view model" display="Model"/>
+    <hyperlink ref="A3" location="'Taxon'!A1" tooltip="Click to view taxon" display="Taxon"/>
+    <hyperlink ref="A4" location="'Environment'!A1" tooltip="Click to view environment" display="Environment"/>
+    <hyperlink ref="A5" location="'Submodels'!A1" tooltip="Click to view submodels" display="Submodels"/>
+    <hyperlink ref="A6" location="'Compartments'!A1" tooltip="Click to view compartments" display="Compartments"/>
+    <hyperlink ref="A7" location="'Species types'!A1" tooltip="Click to view species types" display="Species types"/>
+    <hyperlink ref="A8" location="'Species'!A1" tooltip="Click to view species" display="Species"/>
+    <hyperlink ref="A9" location="'Initial species concentrations'!A1" tooltip="Click to view initial species concentrations" display="Initial species concentrations"/>
+    <hyperlink ref="A10" location="'Observables'!A1" tooltip="Click to view observables" display="Observables"/>
+    <hyperlink ref="A11" location="'Functions'!A1" tooltip="Click to view functions" display="Functions"/>
+    <hyperlink ref="A12" location="'Reactions'!A1" tooltip="Click to view reactions" display="Reactions"/>
+    <hyperlink ref="A13" location="'Rate laws'!A1" tooltip="Click to view rate laws" display="Rate laws"/>
+    <hyperlink ref="A14" location="'dFBA objectives'!A1" tooltip="Click to view dfba objectives" display="dFBA objectives"/>
+    <hyperlink ref="A15" location="'dFBA objective reactions'!A1" tooltip="Click to view dfba objective reactions" display="dFBA objective reactions"/>
+    <hyperlink ref="A16" location="'dFBA objective species'!A1" tooltip="Click to view dfba objective species" display="dFBA objective species"/>
+    <hyperlink ref="A17" location="'Parameters'!A1" tooltip="Click to view parameters" display="Parameters"/>
+    <hyperlink ref="A18" location="'Stop conditions'!A1" tooltip="Click to view stop conditions" display="Stop conditions"/>
+    <hyperlink ref="A19" location="'Observations'!A1" tooltip="Click to view observations" display="Observations"/>
+    <hyperlink ref="A20" location="'Observation sets'!A1" tooltip="Click to view observation sets" display="Observation sets"/>
+    <hyperlink ref="A21" location="'Conclusions'!A1" tooltip="Click to view conclusions" display="Conclusions"/>
+    <hyperlink ref="A22" location="'References'!A1" tooltip="Click to view references" display="References"/>
+    <hyperlink ref="A23" location="'Authors'!A1" tooltip="Click to view authors" display="Authors"/>
+    <hyperlink ref="A24" location="'Changes'!A1" tooltip="Click to view changes" display="Changes"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3340,21 +3340,21 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="9" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="10" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="9"/>
+    <col hidden="1" width="9" customWidth="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Observable' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Observable' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -3408,26 +3408,26 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="I1:I2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="H1:H2" type="textLength">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="G1:G2"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="F1:F2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="list">
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." type="list" errorStyle="warning">
       <formula1>"molecule"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="E1:E2"/>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a linear expression of Observables and Species." errorStyle="warning" errorTitle="Expression" prompt="Enter a linear expression of Observables and Species." promptTitle="Expression" showErrorMessage="1" showInputMessage="1" sqref="C1:C2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Expression" error="Value must be a linear expression of Observables and Species." promptTitle="Expression" prompt="Enter a linear expression of Observables and Species." errorStyle="warning"/>
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -3441,21 +3441,21 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="9" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="10" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="9"/>
+    <col hidden="1" width="9" customWidth="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Function' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Function' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -3532,24 +3532,24 @@
   </sheetData>
   <autoFilter ref="A1:I2"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="I2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="H2" type="textLength">
+    <dataValidation sqref="I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="G2"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="F2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="E2"/>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2" type="textLength">
+    <dataValidation sqref="G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning" errorTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" showErrorMessage="1" showInputMessage="1" sqref="C2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="D2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2" type="textLength">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning"/>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." errorStyle="warning"/>
+    <dataValidation sqref="B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -3563,21 +3563,21 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="14" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="15" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="14"/>
+    <col hidden="1" width="9" customWidth="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reaction' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Reaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4057,42 +4057,42 @@
     <mergeCell ref="G2:I2"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="M3:M12" type="textLength">
+    <dataValidation sqref="M3:M12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="L3:L12"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="K3:K12"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="N3:N12"/>
-    <dataValidation allowBlank="0" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." errorStyle="warning" errorTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" showErrorMessage="1" showInputMessage="1" sqref="E3:E12" type="list">
+    <dataValidation sqref="L3:L12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="K3:K12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="N3:N12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="E3:E12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Reversible" error="Enter a Boolean value&#10;&#10;Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="Reversible" prompt="Enter a Boolean value&#10;&#10;Select &quot;True&quot; or &quot;False&quot;." type="list" errorStyle="warning">
       <formula1>"True,False"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="J3:J12"/>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Maximum" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Maximum" showErrorMessage="1" showInputMessage="1" sqref="H3:H12" type="decimal">
+    <dataValidation sqref="J3:J12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="H3:H12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Maximum" error="Value must be a float or blank." promptTitle="Maximum" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Minimum" operator="between" prompt="Enter a float or blank." promptTitle="Minimum" showErrorMessage="1" showInputMessage="1" sqref="G3:G12" type="decimal">
+    <dataValidation sqref="G3:G12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Minimum" error="Value must be a float or blank." promptTitle="Minimum" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." errorStyle="warning" errorTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" showErrorMessage="1" showInputMessage="1" sqref="F3:F12" type="list">
+    <dataValidation sqref="F3:F12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" errorStyle="warning" errorTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" showErrorMessage="1" showInputMessage="1" sqref="D3:D12"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="I3:I12" type="list">
+    <dataValidation sqref="D3:D12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Participants" error="Value must be a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" promptTitle="Participants" prompt="Enter a reaction string using species from &quot;Species:A&quot;.&#10;&#10;Examples:&#10;* [c]: atp + h2o ==&gt; adp + pi + h&#10;* glc[e] + atp[c] + h2o[c] ==&gt; glc[e] + adp[c] + pi[c] + h[c]&#10;* (3) Na[c] + (2) K[e] ==&gt; (3) Na[e] + (2) K[c]" errorStyle="warning"/>
+    <dataValidation sqref="I3:I12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"molar / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A3:A12" type="textLength">
+    <dataValidation sqref="A3:A12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Submodels:A&quot; or blank." errorStyle="warning" errorTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" showErrorMessage="1" showInputMessage="1" sqref="C3:C12" type="list">
+    <dataValidation sqref="C3:C12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Submodels!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B3:B12" type="textLength">
+    <dataValidation sqref="B3:B12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -4106,21 +4106,21 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="12" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="13" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="12"/>
+    <col hidden="1" width="9" customWidth="1" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='RateLaw' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='RateLaw' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4529,34 +4529,34 @@
   </sheetData>
   <autoFilter ref="A1:L11"/>
   <dataValidations count="12">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A11" type="textLength">
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="K2:K11" type="textLength">
+    <dataValidation sqref="K2:K11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="E2:E11" type="list">
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;Michaelis_Menten_rate_law&quot;, &quot;hill_rate_law&quot;, &quot;mass_action_rate_law&quot;, &quot;modular_rate_law&quot; or blank." type="list" errorStyle="warning">
       <formula1>"Michaelis_Menten_rate_law,hill_rate_law,mass_action_rate_law,modular_rate_law"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="I2:I11"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="L2:L11"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="H2:H11"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="G2:G11" type="list">
+    <dataValidation sqref="I2:I11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="L2:L11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H2:H11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="G2:G11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="J2:J11"/>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Reactions:A&quot; or blank." errorStyle="warning" errorTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" showErrorMessage="1" showInputMessage="1" sqref="C2:C11" type="list">
+    <dataValidation sqref="J2:J11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="C2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Reaction" error="Value must be a value from &quot;Reactions:A&quot; or blank." promptTitle="Reaction" prompt="Select a value from &quot;Reactions:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Reactions!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning" errorTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" showErrorMessage="1" showInputMessage="1" sqref="F2:F11"/>
-    <dataValidation allowBlank="0" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." errorStyle="warning" errorTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" showErrorMessage="1" showInputMessage="1" sqref="D2:D11" type="list">
+    <dataValidation sqref="F2:F11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning"/>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Direction" error="Value must be one of &quot;backward&quot;, &quot;forward&quot;." promptTitle="Direction" prompt="Select one of &quot;backward&quot;, &quot;forward&quot;." type="list" errorStyle="warning">
       <formula1>"backward,forward"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B11" type="textLength">
+    <dataValidation sqref="B2:B11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -4570,21 +4570,21 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="12" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="13" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="12"/>
+    <col hidden="1" width="9" customWidth="1" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjective' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DfbaObjective' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4653,34 +4653,34 @@
   </sheetData>
   <autoFilter ref="A1:L1"/>
   <dataValidations count="12">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="list">
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." type="list" errorStyle="warning">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="K1:K2" type="textLength">
+    <dataValidation sqref="K1:K2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="I1:I2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="L1:L2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="H1:H2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." errorStyle="warning" errorTitle="Reaction rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." promptTitle="Reaction rate units" showErrorMessage="1" showInputMessage="1" sqref="F1:F2" type="list">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="L1:L2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Reaction rate units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Reaction rate units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;second&quot; or blank." errorStyle="warning" errorTitle="Coefficient units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;second&quot; or blank." promptTitle="Coefficient units" showErrorMessage="1" showInputMessage="1" sqref="G1:G2" type="list">
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Coefficient units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;second&quot; or blank." promptTitle="Coefficient units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="J1:J2"/>
-    <dataValidation allowBlank="0" error="Value must be a expression of dFBA objective reactions and Reactions." errorStyle="warning" errorTitle="Expression" prompt="Enter a expression of dFBA objective reactions and Reactions." promptTitle="Expression" showErrorMessage="1" showInputMessage="1" sqref="D1:D2"/>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Submodels:A&quot;." errorStyle="warning" errorTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot;." promptTitle="Submodel" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="list">
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Expression" error="Value must be a expression of dFBA objective reactions and Reactions." promptTitle="Expression" prompt="Enter a expression of dFBA objective reactions and Reactions." errorStyle="warning"/>
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot;." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot;." type="list" errorStyle="warning">
       <formula1>Submodels!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -4694,21 +4694,21 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="10" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="11" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="10"/>
+    <col hidden="1" width="9" customWidth="1" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjReaction' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DfbaObjReaction' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4767,31 +4767,31 @@
   </sheetData>
   <autoFilter ref="A1:J1"/>
   <dataValidations count="10">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="I1:I2" type="textLength">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="H1:H2"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="G1:G2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="F1:F2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="J1:J2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;liter&quot;, &quot;gDCW&quot; or blank." errorStyle="warning" errorTitle="Cell size units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;liter&quot;, &quot;gDCW&quot; or blank." promptTitle="Cell size units" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="list">
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Cell size units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;liter&quot;, &quot;gDCW&quot; or blank." promptTitle="Cell size units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;liter&quot;, &quot;gDCW&quot; or blank." type="list" errorStyle="warning">
       <formula1>"liter,gDCW"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Submodels:A&quot; or blank." errorStyle="warning" errorTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="list">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Submodels!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="list">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;1 / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;1 / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"1 / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -4805,21 +4805,21 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="11" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="12" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="11"/>
+    <col hidden="1" width="9" customWidth="1" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DfbaObjSpecies' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DfbaObjSpecies' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -4883,34 +4883,34 @@
   </sheetData>
   <autoFilter ref="A1:K1"/>
   <dataValidations count="11">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="J1:J2" type="textLength">
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="I1:I2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="G1:G2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot;, &quot;mole / gDCW / second&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot;, &quot;mole / gDCW / second&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="F1:F2" type="list">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molar / second&quot;, &quot;mole / gDCW / second&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molar / second&quot;, &quot;mole / gDCW / second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"molar / second,mole / gDCW / second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Species:A&quot;." errorStyle="warning" errorTitle="Species" prompt="Select a value from &quot;Species:A&quot;." promptTitle="Species" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="list">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." type="list" errorStyle="warning">
       <formula1>Species!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="H1:H2"/>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Value" operator="between" prompt="Enter a float or blank." promptTitle="Value" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="decimal">
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;dFBA objective reactions:A&quot;." errorStyle="warning" errorTitle="dFBA objective reaction" prompt="Select a value from &quot;dFBA objective reactions:A&quot;." promptTitle="dFBA objective reaction" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="list">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="dFBA objective reaction" error="Value must be a value from &quot;dFBA objective reactions:A&quot;." promptTitle="dFBA objective reaction" prompt="Select a value from &quot;dFBA objective reactions:A&quot;." type="list" errorStyle="warning">
       <formula1>'dFBA objective reactions'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="K1:K2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="K1:K2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -4924,21 +4924,21 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="11" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="12" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="11"/>
+    <col hidden="1" width="9" customWidth="1" min="12" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Parameter' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Parameter' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5734,33 +5734,33 @@
   </sheetData>
   <autoFilter ref="A1:K29"/>
   <dataValidations count="11">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="J2:J29" type="textLength">
+    <dataValidation sqref="J2:J29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="I2:I29"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="G2:G29"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="H2:H29"/>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Value" operator="between" prompt="Enter a float or blank." promptTitle="Value" showErrorMessage="1" showInputMessage="1" sqref="D2:D29" type="decimal">
+    <dataValidation sqref="I2:I29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="G2:G29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="H2:H29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="D2:D29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Value" error="Value must be a float or blank." promptTitle="Value" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="C2:C29" type="list">
+    <dataValidation sqref="C2:C29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;kinetic_constant&quot;, &quot;K_i&quot;, &quot;K_m&quot;, &quot;k_cat&quot;, &quot;v_max&quot; or blank." type="list" errorStyle="warning">
       <formula1>"kinetic_constant,K_i,K_m,k_cat,v_max"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="K2:K29"/>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Standard error" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Standard error" showErrorMessage="1" showInputMessage="1" sqref="E2:E29" type="decimal">
+    <dataValidation sqref="K2:K29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="E2:E29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Standard error" error="Value must be a float or blank." promptTitle="Standard error" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B29" type="textLength">
+    <dataValidation sqref="B2:B29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="F2:F29"/>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A29" type="textLength">
+    <dataValidation sqref="F2:F29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." errorStyle="warning"/>
+    <dataValidation sqref="A2:A29" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -5774,21 +5774,21 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="9" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="10" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="9"/>
+    <col hidden="1" width="9" customWidth="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='StopCondition' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -5842,26 +5842,26 @@
   </sheetData>
   <autoFilter ref="A1:I1"/>
   <dataValidations count="9">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="I1:I2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="H1:H2" type="textLength">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="F1:F2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="E1:E2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="G1:G2"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="list">
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." type="list" errorStyle="warning">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning" errorTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" showErrorMessage="1" showInputMessage="1" sqref="C1:C2"/>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Expression" error="Value must be a expression of Compartments, Functions, Observables, Parameters and Species." promptTitle="Expression" prompt="Enter a expression of Compartments, Functions, Observables, Parameters and Species." errorStyle="warning"/>
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -5875,21 +5875,21 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="23" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="24" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="23"/>
+    <col hidden="1" width="9" customWidth="1" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Observation' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6052,68 +6052,68 @@
     <mergeCell ref="S2:T2"/>
   </mergeCells>
   <dataValidations count="21">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="V2:V3" type="textLength">
+    <dataValidation sqref="V2:V3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="W2:W3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="U2:U3"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Version" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Version" showErrorMessage="1" showInputMessage="1" sqref="R2:R3 T2:T3" type="textLength">
+    <dataValidation sqref="W2:W3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="U2:U3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="R2:R3 T2:T3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Version" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Version" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Experiment type" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Experiment type" showErrorMessage="1" showInputMessage="1" sqref="O2:O3" type="textLength">
+    <dataValidation sqref="O2:O3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Experiment type" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Experiment type" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Condition" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Condition" showErrorMessage="1" showInputMessage="1" sqref="N2:N3" type="textLength">
+    <dataValidation sqref="N2:N3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Condition" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Condition" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Growth media" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Growth media" showErrorMessage="1" showInputMessage="1" sqref="M2:M3" type="textLength">
+    <dataValidation sqref="M2:M3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Growth media" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Growth media" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." errorStyle="warning" errorTitle="pH units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." promptTitle="pH units" showErrorMessage="1" showInputMessage="1" sqref="L2:L3" type="list">
+    <dataValidation sqref="L2:L3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="pH units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="pH units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." type="list" errorStyle="warning">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="pH" operator="between" prompt="Enter a float or blank." promptTitle="pH" showErrorMessage="1" showInputMessage="1" sqref="K2:K3" type="decimal">
+    <dataValidation sqref="K2:K3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="pH" error="Value must be a float or blank." promptTitle="pH" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="Q2:Q3 S2:S3" type="textLength">
+    <dataValidation sqref="Q2:Q3 S2:S3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Temperature" operator="between" prompt="Enter a float or blank." promptTitle="Temperature" showErrorMessage="1" showInputMessage="1" sqref="I2:I3" type="decimal">
+    <dataValidation sqref="I2:I3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Temperature" error="Value must be a float or blank." promptTitle="Temperature" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Taxon" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Taxon" showErrorMessage="1" showInputMessage="1" sqref="G2:G3" type="textLength">
+    <dataValidation sqref="G2:G3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Taxon" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Taxon" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Experiment design" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Experiment design" showErrorMessage="1" showInputMessage="1" sqref="P2:P3" type="textLength">
+    <dataValidation sqref="P2:P3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Experiment design" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Experiment design" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;degC&quot; or blank." errorStyle="warning" errorTitle="Temperature units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;degC&quot; or blank." promptTitle="Temperature units" showErrorMessage="1" showInputMessage="1" sqref="J2:J3" type="list">
+    <dataValidation sqref="J2:J3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Temperature units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;degC&quot; or blank." promptTitle="Temperature units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;degC&quot; or blank." type="list" errorStyle="warning">
       <formula1>"degC"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;computational_observation&quot;, &quot;experimental_observation&quot;, &quot;theoretical_observation&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;computational_observation&quot;, &quot;experimental_observation&quot;, &quot;theoretical_observation&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="F2:F3" type="list">
+    <dataValidation sqref="F2:F3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;computational_observation&quot;, &quot;experimental_observation&quot;, &quot;theoretical_observation&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;computational_observation&quot;, &quot;experimental_observation&quot;, &quot;theoretical_observation&quot; or blank." type="list" errorStyle="warning">
       <formula1>"computational_observation,experimental_observation,theoretical_observation"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Value" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Value" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="textLength">
+    <dataValidation sqref="C2:C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Variant" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Variant" showErrorMessage="1" showInputMessage="1" sqref="H2:H3" type="textLength">
+    <dataValidation sqref="H2:H3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Variant" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Variant" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Standard error" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Standard error" showErrorMessage="1" showInputMessage="1" sqref="D2:D3" type="textLength">
+    <dataValidation sqref="D2:D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Standard error" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Standard error" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A3" type="textLength">
+    <dataValidation sqref="A2:A3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="E2:E3"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B3" type="textLength">
+    <dataValidation sqref="E2:E3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." errorStyle="warning"/>
+    <dataValidation sqref="B2:B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6127,21 +6127,21 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="2" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="3" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="2"/>
+    <col hidden="1" width="9" customWidth="1" min="3" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Model' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Model' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -6271,41 +6271,41 @@
     </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation allowBlank="0" error="Value must be a date and time." errorStyle="warning" errorTitle="Updated" operator="between" prompt="Enter a date and time." promptTitle="Updated" showErrorMessage="1" showInputMessage="1" sqref="B12" type="date">
+    <dataValidation sqref="B12" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Updated" error="Value must be a date and time." promptTitle="Updated" prompt="Enter a date and time." type="date" errorStyle="warning" operator="between">
       <formula1>0</formula1>
       <formula2>-328717</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="B10" type="textLength">
+    <dataValidation sqref="B10" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Branch" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Branch" showErrorMessage="1" showInputMessage="1" sqref="B5" type="textLength">
+    <dataValidation sqref="B5" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Branch" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="B9"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;second&quot; or blank." errorStyle="warning" errorTitle="Time units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;second&quot; or blank." promptTitle="Time units" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
+    <dataValidation sqref="B9" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="B8" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Time units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;second&quot; or blank." promptTitle="Time units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;second&quot; or blank." type="list" errorStyle="warning">
       <formula1>"second"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string." errorStyle="warning" errorTitle="wc_lang version" prompt="Enter a string." promptTitle="wc_lang version" showErrorMessage="1" showInputMessage="1" sqref="B7"/>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="B1" type="textLength">
+    <dataValidation sqref="B7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="wc_lang version" error="Value must be a string." promptTitle="wc_lang version" prompt="Enter a string." errorStyle="warning"/>
+    <dataValidation sqref="B1" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a valid URL&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 65535 characters." errorStyle="warning" errorTitle="URL" operator="lessThanOrEqual" prompt="Enter a valid URL&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 65535 characters." promptTitle="URL" showErrorMessage="1" showInputMessage="1" sqref="B4" type="textLength">
+    <dataValidation sqref="B4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="URL" error="Enter a valid URL&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 65535 characters." promptTitle="URL" prompt="Enter a valid URL&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 65535 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>65535</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string." errorStyle="warning" errorTitle="Version" prompt="Enter a string." promptTitle="Version" showErrorMessage="1" showInputMessage="1" sqref="B3"/>
-    <dataValidation allowBlank="0" error="Value must be a date and time." errorStyle="warning" errorTitle="Created" operator="between" prompt="Enter a date and time." promptTitle="Created" showErrorMessage="1" showInputMessage="1" sqref="B11" type="date">
+    <dataValidation sqref="B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Version" error="Value must be a string." promptTitle="Version" prompt="Enter a string." errorStyle="warning"/>
+    <dataValidation sqref="B11" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Created" error="Value must be a date and time." promptTitle="Created" prompt="Enter a date and time." type="date" errorStyle="warning" operator="between">
       <formula1>0</formula1>
       <formula2>-328717</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2" type="textLength">
+    <dataValidation sqref="B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Revision" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Revision" showErrorMessage="1" showInputMessage="1" sqref="B6" type="textLength">
+    <dataValidation sqref="B6" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Revision" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Revision" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6319,21 +6319,21 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="6" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="7" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="6"/>
+    <col hidden="1" width="9" customWidth="1" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='ObservationSet' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='ObservationSet' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6372,21 +6372,21 @@
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <dataValidations count="6">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="F1:F2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="textLength">
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="D1:D2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Observations:A&quot; or blank." errorStyle="warning" errorTitle="Observations" prompt="Enter a comma-separated list of values from &quot;Observations:A&quot; or blank." promptTitle="Observations" showErrorMessage="1" showInputMessage="1" sqref="C1:C2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Observations" error="Value must be a comma-separated list of values from &quot;Observations:A&quot; or blank." promptTitle="Observations" prompt="Enter a comma-separated list of values from &quot;Observations:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6400,21 +6400,21 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="14" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="15" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="14"/>
+    <col hidden="1" width="9" customWidth="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Conclusion' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Conclusion' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6515,42 +6515,42 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Authors:A&quot; or blank." errorStyle="warning" errorTitle="Authors" prompt="Enter a comma-separated list of values from &quot;Authors:A&quot; or blank." promptTitle="Authors" showErrorMessage="1" showInputMessage="1" sqref="M2:M3"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="K2:K3" type="textLength">
+    <dataValidation sqref="M2:M3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Authors" error="Value must be a comma-separated list of values from &quot;Authors:A&quot; or blank." promptTitle="Authors" prompt="Enter a comma-separated list of values from &quot;Authors:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="K2:K3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="G2:G3" type="textLength">
+    <dataValidation sqref="G2:G3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="J2:J3"/>
-    <dataValidation allowBlank="0" error="Value must be a date and time." errorStyle="warning" errorTitle="Date" operator="between" prompt="Enter a date and time." promptTitle="Date" showErrorMessage="1" showInputMessage="1" sqref="N2:N3" type="date">
+    <dataValidation sqref="J2:J3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="N2:N3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Date" error="Value must be a date and time." promptTitle="Date" prompt="Enter a date and time." type="date" errorStyle="warning" operator="between">
       <formula1>0</formula1>
       <formula2>-328717</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="L2:L3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="I2:I3"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Version" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Version" showErrorMessage="1" showInputMessage="1" sqref="H2:H3" type="textLength">
+    <dataValidation sqref="L2:L3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="I2:I3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="H2:H3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Version" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Version" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Standard error" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Standard error" showErrorMessage="1" showInputMessage="1" sqref="D2:D3" type="textLength">
+    <dataValidation sqref="D2:D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Standard error" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Standard error" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Value" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Value" showErrorMessage="1" showInputMessage="1" sqref="C2:C3" type="textLength">
+    <dataValidation sqref="C2:C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A3" type="textLength">
+    <dataValidation sqref="A2:A3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="E2:E3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;approximation&quot;, &quot;assumption&quot;, &quot;computation&quot;, &quot;decision&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;approximation&quot;, &quot;assumption&quot;, &quot;computation&quot;, &quot;decision&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="F2:F3" type="list">
+    <dataValidation sqref="E2:E3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be a unit or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Enter a unit or blank." errorStyle="warning"/>
+    <dataValidation sqref="F2:F3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;approximation&quot;, &quot;assumption&quot;, &quot;computation&quot;, &quot;decision&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;approximation&quot;, &quot;assumption&quot;, &quot;computation&quot;, &quot;decision&quot; or blank." type="list" errorStyle="warning">
       <formula1>"approximation,assumption,computation,decision"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B3" type="textLength">
+    <dataValidation sqref="B2:B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6564,21 +6564,21 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="18" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="19" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="18"/>
+    <col hidden="1" width="9" customWidth="1" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Reference' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Reference' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6677,61 +6677,61 @@
   </sheetData>
   <autoFilter ref="A1:R1"/>
   <dataValidations count="18">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="R1:R2" type="textLength">
+    <dataValidation sqref="R1:R2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="Q1:Q2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Edition" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Edition" showErrorMessage="1" showInputMessage="1" sqref="N1:N2" type="textLength">
+    <dataValidation sqref="Q1:Q2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="N1:N2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Edition" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Edition" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Issue" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Issue" showErrorMessage="1" showInputMessage="1" sqref="M1:M2" type="textLength">
+    <dataValidation sqref="M1:M2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Issue" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Issue" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Chapter" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Chapter" showErrorMessage="1" showInputMessage="1" sqref="O1:O2" type="textLength">
+    <dataValidation sqref="O1:O2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Chapter" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Chapter" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Series" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Series" showErrorMessage="1" showInputMessage="1" sqref="J1:J2" type="textLength">
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Series" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Series" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Publication" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publication" showErrorMessage="1" showInputMessage="1" sqref="H1:H2" type="textLength">
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Publication" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publication" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Pages" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Pages" showErrorMessage="1" showInputMessage="1" sqref="P1:P2" type="textLength">
+    <dataValidation sqref="P1:P2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Pages" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Pages" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Author" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Author" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="textLength">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Author" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Author" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;article&quot;, &quot;book&quot;, &quot;preprint&quot;, &quot;proceedings&quot;, &quot;supplementary_material&quot;, &quot;thesis&quot;, &quot;website&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;article&quot;, &quot;book&quot;, &quot;preprint&quot;, &quot;proceedings&quot;, &quot;supplementary_material&quot;, &quot;thesis&quot;, &quot;website&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="G1:G2" type="list">
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;article&quot;, &quot;book&quot;, &quot;preprint&quot;, &quot;proceedings&quot;, &quot;supplementary_material&quot;, &quot;thesis&quot;, &quot;website&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;article&quot;, &quot;book&quot;, &quot;preprint&quot;, &quot;proceedings&quot;, &quot;supplementary_material&quot;, &quot;thesis&quot;, &quot;website&quot; or blank." type="list" errorStyle="warning">
       <formula1>"article,book,preprint,proceedings,supplementary_material,thesis,website"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Title" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Title" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="textLength">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Title" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Title" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Editor" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Editor" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="textLength">
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Editor" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Editor" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Number" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Number" showErrorMessage="1" showInputMessage="1" sqref="L1:L2" type="textLength">
+    <dataValidation sqref="L1:L2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Number" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Number" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Publisher" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publisher" showErrorMessage="1" showInputMessage="1" sqref="I1:I2" type="textLength">
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Publisher" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Publisher" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be an integer." errorStyle="warning" errorTitle="Year" operator="greaterThanOrEqual" prompt="Enter an integer.&#10;&#10;Value must be positive." promptTitle="Year" showErrorMessage="1" showInputMessage="1" sqref="F1:F2" type="whole">
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Year" error="Value must be an integer." promptTitle="Year" prompt="Enter an integer.&#10;&#10;Value must be positive." type="whole" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Volume" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Volume" showErrorMessage="1" showInputMessage="1" sqref="K1:K2" type="textLength">
+    <dataValidation sqref="K1:K2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Volume" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Volume" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6745,21 +6745,21 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="12" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="13" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="12"/>
+    <col hidden="1" width="9" customWidth="1" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Author' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Author' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6828,46 +6828,46 @@
   </sheetData>
   <autoFilter ref="A1:L1"/>
   <dataValidations count="12">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="L1:L2" type="textLength">
+    <dataValidation sqref="L1:L2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="K1:K2"/>
-    <dataValidation allowBlank="0" error="Enter a valid URL&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 65535 characters." errorStyle="warning" errorTitle="Website" operator="lessThanOrEqual" prompt="Enter a valid URL&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 65535 characters." promptTitle="Website" showErrorMessage="1" showInputMessage="1" sqref="I1:I2" type="textLength">
+    <dataValidation sqref="K1:K2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Website" error="Enter a valid URL&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 65535 characters." promptTitle="Website" prompt="Enter a valid URL&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 65535 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>65535</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." errorStyle="warning" errorTitle="Last name" operator="between" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Last name" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="textLength">
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Last name" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Last name" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Organization" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Organization" showErrorMessage="1" showInputMessage="1" sqref="G1:G2" type="textLength">
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Organization" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Organization" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a valid email address&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Email" operator="lessThanOrEqual" prompt="Enter a valid email address&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Email" showErrorMessage="1" showInputMessage="1" sqref="H1:H2" type="textLength">
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Email" error="Enter a valid email address&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Email" prompt="Enter a valid email address&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Title" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Title" showErrorMessage="1" showInputMessage="1" sqref="F1:F2" type="textLength">
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Title" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Title" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." errorStyle="warning" errorTitle="Name" operator="between" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." errorStyle="warning" errorTitle="Middle name" operator="between" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Middle name" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="textLength">
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Middle name" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Middle name" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="First name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="First name" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="textLength">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="First name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="First name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Address" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Address" showErrorMessage="1" showInputMessage="1" sqref="J1:J2" type="textLength">
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Address" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Address" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -6881,21 +6881,21 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="17" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="18" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="17"/>
+    <col hidden="1" width="9" customWidth="1" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Change' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Change' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -6989,52 +6989,52 @@
   </sheetData>
   <autoFilter ref="A1:Q1"/>
   <dataValidations count="17">
-    <dataValidation allowBlank="0" error="Value must be a date and time." errorStyle="warning" errorTitle="Date" operator="between" prompt="Enter a date and time." promptTitle="Date" showErrorMessage="1" showInputMessage="1" sqref="Q1:Q2" type="date">
+    <dataValidation sqref="Q1:Q2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Date" error="Value must be a date and time." promptTitle="Date" prompt="Enter a date and time." type="date" errorStyle="warning" operator="between">
       <formula1>0</formula1>
       <formula2>-328717</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="O1:O2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="K1:K2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Intention" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Intention" showErrorMessage="1" showInputMessage="1" sqref="I1:I2" type="textLength">
+    <dataValidation sqref="O1:O2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="K1:K2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="I1:I2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Intention" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Intention" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Authors:A&quot; or blank." errorStyle="warning" errorTitle="Authors" prompt="Enter a comma-separated list of values from &quot;Authors:A&quot; or blank." promptTitle="Authors" showErrorMessage="1" showInputMessage="1" sqref="P1:P2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;correct_intention_provenance&quot;, &quot;elaborate_intention_provenance&quot;, &quot;expand_intention_provenance&quot;, &quot;simplify_intention_provenance&quot; or blank." errorStyle="warning" errorTitle="Intention type" prompt="Enter a comma-separated list of WC ontology terms &quot;correct_intention_provenance&quot;, &quot;elaborate_intention_provenance&quot;, &quot;expand_intention_provenance&quot;, &quot;simplify_intention_provenance&quot; or blank." promptTitle="Intention type" showErrorMessage="1" showInputMessage="1" sqref="J1:J2" type="list">
+    <dataValidation sqref="P1:P2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Authors" error="Value must be a comma-separated list of values from &quot;Authors:A&quot; or blank." promptTitle="Authors" prompt="Enter a comma-separated list of values from &quot;Authors:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="J1:J2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Intention type" error="Value must be a comma-separated list of WC ontology terms &quot;correct_intention_provenance&quot;, &quot;elaborate_intention_provenance&quot;, &quot;expand_intention_provenance&quot;, &quot;simplify_intention_provenance&quot; or blank." promptTitle="Intention type" prompt="Enter a comma-separated list of WC ontology terms &quot;correct_intention_provenance&quot;, &quot;elaborate_intention_provenance&quot;, &quot;expand_intention_provenance&quot;, &quot;simplify_intention_provenance&quot; or blank." type="list" errorStyle="warning">
       <formula1>"correct_intention_provenance,elaborate_intention_provenance,expand_intention_provenance,simplify_intention_provenance"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Reason" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Reason" showErrorMessage="1" showInputMessage="1" sqref="G1:G2" type="textLength">
+    <dataValidation sqref="G1:G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Reason" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Reason" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="L1:L2"/>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Submodels:A&quot; or blank." errorStyle="warning" errorTitle="Target submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." promptTitle="Target submodel" showErrorMessage="1" showInputMessage="1" sqref="E1:E2" type="list">
+    <dataValidation sqref="L1:L2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="E1:E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Target submodel" error="Value must be a value from &quot;Submodels:A&quot; or blank." promptTitle="Target submodel" prompt="Select a value from &quot;Submodels:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Submodels!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="N1:N2" type="textLength">
+    <dataValidation sqref="N1:N2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Target" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Target" showErrorMessage="1" showInputMessage="1" sqref="D1:D2" type="textLength">
+    <dataValidation sqref="D1:D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Target" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Target" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;add_metadata_reason_provenance&quot;, &quot;implementation_error_reason_provenance&quot;, &quot;incorrect_interpretation_reason_provenance&quot;, &quot;migrate_version_reason_provenance&quot;, &quot;new_goal_reason_provenance&quot;, &quot;new ..." errorStyle="warning" errorTitle="Reason type" prompt="Enter a comma-separated list of WC ontology terms &quot;add_metadata_reason_provenance&quot;, &quot;implementation_error_reason_provenance&quot;, &quot;incorrect_interpretation_reason_provenance&quot;, &quot;migrate_version_reason_provenance&quot;, &quot;new_goal_reason_provenance&quot;, &quot;new_knowled ..." promptTitle="Reason type" showErrorMessage="1" showInputMessage="1" sqref="H1:H2" type="list">
+    <dataValidation sqref="H1:H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Reason type" error="Value must be a comma-separated list of WC ontology terms &quot;add_metadata_reason_provenance&quot;, &quot;implementation_error_reason_provenance&quot;, &quot;incorrect_interpretation_reason_provenance&quot;, &quot;migrate_version_reason_provenance&quot;, &quot;new_goal_reason_provenance&quot;, &quot;new ..." promptTitle="Reason type" prompt="Enter a comma-separated list of WC ontology terms &quot;add_metadata_reason_provenance&quot;, &quot;implementation_error_reason_provenance&quot;, &quot;incorrect_interpretation_reason_provenance&quot;, &quot;migrate_version_reason_provenance&quot;, &quot;new_goal_reason_provenance&quot;, &quot;new_knowled ..." type="list" errorStyle="warning">
       <formula1>"add_metadata_reason_provenance,implementation_error_reason_provenance,incorrect_interpretation_reason_provenance,migrate_version_reason_provenance,new_goal_reason_provenance,new_knowledge_reason_provenance"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;data_target_provenance&quot;, &quot;encoding_target_provenance&quot;, &quot;metadata_target_provenance&quot;, &quot;model_target_provenance&quot;, &quot;model_dynamics_target_provenance&quot;, &quot;model_initial_conditions_target_provenance&quot; ..." errorStyle="warning" errorTitle="Target type" prompt="Enter a comma-separated list of WC ontology terms &quot;data_target_provenance&quot;, &quot;encoding_target_provenance&quot;, &quot;metadata_target_provenance&quot;, &quot;model_target_provenance&quot;, &quot;model_dynamics_target_provenance&quot;, &quot;model_initial_conditions_target_provenance&quot; or blank." promptTitle="Target type" showErrorMessage="1" showInputMessage="1" sqref="F1:F2" type="list">
+    <dataValidation sqref="F1:F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Target type" error="Value must be a comma-separated list of WC ontology terms &quot;data_target_provenance&quot;, &quot;encoding_target_provenance&quot;, &quot;metadata_target_provenance&quot;, &quot;model_target_provenance&quot;, &quot;model_dynamics_target_provenance&quot;, &quot;model_initial_conditions_target_provenance&quot; ..." promptTitle="Target type" prompt="Enter a comma-separated list of WC ontology terms &quot;data_target_provenance&quot;, &quot;encoding_target_provenance&quot;, &quot;metadata_target_provenance&quot;, &quot;model_target_provenance&quot;, &quot;model_dynamics_target_provenance&quot;, &quot;model_initial_conditions_target_provenance&quot; or blank." type="list" errorStyle="warning">
       <formula1>"data_target_provenance,encoding_target_provenance,metadata_target_provenance,model_target_provenance,model_dynamics_target_provenance,model_initial_conditions_target_provenance"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="M1:M2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;copy&quot;, &quot;deletion_change_provenance&quot;, &quot;insertion&quot;, &quot;merge&quot;, &quot;move&quot;, &quot;revert&quot;, &quot;update&quot; or blank." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;copy&quot;, &quot;deletion_change_provenance&quot;, &quot;insertion&quot;, &quot;merge&quot;, &quot;move&quot;, &quot;revert&quot;, &quot;update&quot; or blank." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="C1:C2" type="list">
+    <dataValidation sqref="M1:M2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="C1:C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;copy&quot;, &quot;deletion_change_provenance&quot;, &quot;insertion&quot;, &quot;merge&quot;, &quot;move&quot;, &quot;revert&quot;, &quot;update&quot; or blank." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;copy&quot;, &quot;deletion_change_provenance&quot;, &quot;insertion&quot;, &quot;merge&quot;, &quot;move&quot;, &quot;revert&quot;, &quot;update&quot; or blank." type="list" errorStyle="warning">
       <formula1>"copy,deletion_change_provenance,insertion,merge,move,revert,update"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." errorStyle="warning" errorTitle="Name" operator="between" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B1:B2" type="textLength">
+    <dataValidation sqref="B1:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be between 1 and 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be between 1 and 255 characters." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:A2" type="textLength">
+    <dataValidation sqref="A1:A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -7048,21 +7048,21 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="2" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="1"/>
+    <col hidden="1" width="9" customWidth="1" min="2" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Taxon' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Taxon' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -7110,20 +7110,20 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="A6:B6"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" prompt="Enter a string.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:B1"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="A5:B5" type="textLength">
+    <dataValidation sqref="A6:B6" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="A1:B1" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be unique." errorStyle="warning"/>
+    <dataValidation sqref="A5:B5" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be one of &quot;domain&quot;, &quot;kingdom&quot;, &quot;phylum&quot;, &quot;classis&quot;, &quot;order&quot;, &quot;family&quot;, &quot;tribe&quot;, &quot;genus&quot;, &quot;species&quot;, &quot;variety&quot;." errorStyle="warning" errorTitle="Rank" prompt="Select one of &quot;domain&quot;, &quot;kingdom&quot;, &quot;phylum&quot;, &quot;classis&quot;, &quot;order&quot;, &quot;family&quot;, &quot;tribe&quot;, &quot;genus&quot;, &quot;species&quot;, &quot;variety&quot;." promptTitle="Rank" showErrorMessage="1" showInputMessage="1" sqref="A3:B3" type="list">
+    <dataValidation sqref="A3:B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Rank" error="Value must be one of &quot;domain&quot;, &quot;kingdom&quot;, &quot;phylum&quot;, &quot;classis&quot;, &quot;order&quot;, &quot;family&quot;, &quot;tribe&quot;, &quot;genus&quot;, &quot;species&quot;, &quot;variety&quot;." promptTitle="Rank" prompt="Select one of &quot;domain&quot;, &quot;kingdom&quot;, &quot;phylum&quot;, &quot;classis&quot;, &quot;order&quot;, &quot;family&quot;, &quot;tribe&quot;, &quot;genus&quot;, &quot;species&quot;, &quot;variety&quot;." type="list" errorStyle="warning">
       <formula1>"domain,kingdom,phylum,classis,order,family,tribe,genus,species,variety"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="A2:B2" type="textLength">
+    <dataValidation sqref="A2:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="A4:B4"/>
+    <dataValidation sqref="A4:B4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -7137,21 +7137,21 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="topRight" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="6"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="2" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="1"/>
+    <col hidden="1" width="9" customWidth="1" min="2" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Environment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Environment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='column'</t>
         </is>
       </c>
     </row>
@@ -7206,24 +7206,24 @@
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="A7:B7"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;degC&quot; or blank." errorStyle="warning" errorTitle="Temperature units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;degC&quot; or blank." promptTitle="Temperature units" showErrorMessage="1" showInputMessage="1" sqref="A4:B4" type="list">
+    <dataValidation sqref="A7:B7" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="A4:B4" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Temperature units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;degC&quot; or blank." promptTitle="Temperature units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;degC&quot; or blank." type="list" errorStyle="warning">
       <formula1>"degC"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Temperature" operator="between" prompt="Enter a float or blank." promptTitle="Temperature" showErrorMessage="1" showInputMessage="1" sqref="A3:B3" type="decimal">
+    <dataValidation sqref="A3:B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Temperature" error="Value must be a float or blank." promptTitle="Temperature" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="A2:B2" type="textLength">
+    <dataValidation sqref="A2:B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="A5:B5"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="A6:B6" type="textLength">
+    <dataValidation sqref="A5:B5" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="A6:B6" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" prompt="Enter a string.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A1:B1"/>
+    <dataValidation sqref="A1:B1" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be unique." errorStyle="warning"/>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -7237,21 +7237,21 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="1"/>
   <cols>
-    <col customWidth="1" max="8" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="9" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="8"/>
+    <col hidden="1" width="9" customWidth="1" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Submodel' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Submodel' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -7318,25 +7318,25 @@
   </sheetData>
   <autoFilter ref="A1:H2"/>
   <dataValidations count="8">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="H2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="F2"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="D2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2" type="textLength">
+    <dataValidation sqref="H2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="F2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="B2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="E2"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="G2" type="textLength">
+    <dataValidation sqref="E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." errorStyle="warning" errorTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" showErrorMessage="1" showInputMessage="1" sqref="C2" type="list">
+    <dataValidation sqref="C2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." type="list" errorStyle="warning">
       <formula1>"dynamic_flux_balance_analysis,ordinary_differential_equations,stochastic_simulation_algorithm"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2" type="textLength">
+    <dataValidation sqref="A2" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -7350,21 +7350,21 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelRow="2"/>
   <cols>
-    <col customWidth="1" max="21" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="22" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="21"/>
+    <col hidden="1" width="9" customWidth="1" min="22" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Compartment' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Compartment' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -7582,57 +7582,57 @@
     <mergeCell ref="M2:P2"/>
   </mergeCells>
   <dataValidations count="19">
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="R3"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="T3" type="textLength">
+    <dataValidation sqref="R3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="T3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="P3" type="list">
+    <dataValidation sqref="P3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;dimensionless&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;dimensionless&quot; or blank." type="list" errorStyle="warning">
       <formula1>"dimensionless"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Mean" operator="between" prompt="Enter a float or blank." promptTitle="Mean" showErrorMessage="1" showInputMessage="1" sqref="N3" type="decimal">
+    <dataValidation sqref="N3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank." type="decimal" errorStyle="warning" operator="between">
       <formula1>-1E+100</formula1>
       <formula2>1E+100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Parameters:A&quot; or blank." errorStyle="warning" errorTitle="Initial density" prompt="Select a value from &quot;Parameters:A&quot; or blank." promptTitle="Initial density" showErrorMessage="1" showInputMessage="1" sqref="L3" type="list">
+    <dataValidation sqref="L3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Initial density" error="Value must be a value from &quot;Parameters:A&quot; or blank." promptTitle="Initial density" prompt="Select a value from &quot;Parameters:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Parameters!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;liter&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;liter&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="K3" type="list">
+    <dataValidation sqref="K3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;liter&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;liter&quot; or blank." type="list" errorStyle="warning">
       <formula1>"liter"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Standard deviation" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Standard deviation" showErrorMessage="1" showInputMessage="1" sqref="J3 O3" type="decimal">
+    <dataValidation sqref="J3 O3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Mean" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Mean" showErrorMessage="1" showInputMessage="1" sqref="I3" type="decimal">
+    <dataValidation sqref="I3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="S3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." errorStyle="warning" errorTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." promptTitle="Distribution" showErrorMessage="1" showInputMessage="1" sqref="H3 M3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="U3"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="Q3"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;gram&quot; or blank." errorStyle="warning" errorTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;gram&quot; or blank." promptTitle="Mass units" showErrorMessage="1" showInputMessage="1" sqref="G3" type="list">
+    <dataValidation sqref="S3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="H3 M3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." errorStyle="warning"/>
+    <dataValidation sqref="U3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="Q3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="G3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Mass units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;gram&quot; or blank." promptTitle="Mass units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;gram&quot; or blank." type="list" errorStyle="warning">
       <formula1>"gram"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Compartments:A&quot; or blank." errorStyle="warning" errorTitle="Parent compartment" prompt="Select a value from &quot;Compartments:A&quot; or blank." promptTitle="Parent compartment" showErrorMessage="1" showInputMessage="1" sqref="F3" type="list">
+    <dataValidation sqref="F3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Parent compartment" error="Value must be a value from &quot;Compartments:A&quot; or blank." promptTitle="Parent compartment" prompt="Select a value from &quot;Compartments:A&quot; or blank." type="list" errorStyle="warning">
       <formula1>Compartments!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." errorStyle="warning" errorTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" showErrorMessage="1" showInputMessage="1" sqref="E3" type="list">
+    <dataValidation sqref="E3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." type="list" errorStyle="warning">
       <formula1>"3D_compartment"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." errorStyle="warning" errorTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" showErrorMessage="1" showInputMessage="1" sqref="D3" type="list">
+    <dataValidation sqref="D3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." type="list" errorStyle="warning">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." errorStyle="warning" errorTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" showErrorMessage="1" showInputMessage="1" sqref="C3" type="list">
+    <dataValidation sqref="C3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." type="list" errorStyle="warning">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B3" type="textLength">
+    <dataValidation sqref="B3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A3" type="textLength">
+    <dataValidation sqref="A3" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -7646,21 +7646,21 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="14" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="15" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="14"/>
+    <col hidden="1" width="9" customWidth="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='SpeciesType' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='SpeciesType' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -8553,40 +8553,40 @@
     <mergeCell ref="C2:H2"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="M3:M22" type="textLength">
+    <dataValidation sqref="M3:M22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="K3:K22"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." errorStyle="warning" errorTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." promptTitle="Type" showErrorMessage="1" showInputMessage="1" sqref="I3:I22"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="L3:L22"/>
-    <dataValidation allowBlank="0" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." errorStyle="warning" errorTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" showErrorMessage="1" showInputMessage="1" sqref="D3:D22" type="list">
+    <dataValidation sqref="K3:K22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="I3:I22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Type" error="Value must be a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;I ..." promptTitle="Type" prompt="Enter a comma-separated list of WC ontology terms &quot;DNA&quot;, &quot;RNA&quot;, &quot;complex&quot;, &quot;metabolite&quot;, &quot;protein&quot;, &quot;pseudo_species&quot;, &quot;asRNA&quot;, &quot;intergenic&quot;, &quot;mRNA&quot;, &quot;mixed&quot;, &quot;ncRNA&quot;, &quot;rRNA&quot;, &quot;sRNA&quot;, &quot;tRNA&quot;, &quot;TRNASynthClassIIComplex&quot;, &quot;fattyAcylAcpComplex&quot;, &quot;Ion&quot;, &quot;am ..." errorStyle="warning"/>
+    <dataValidation sqref="L3:L22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="D3:D22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Format" error="Value must be one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." promptTitle="Format" prompt="Select one of &quot;smiles&quot;, &quot;bpforms&quot; or blank." type="list" errorStyle="warning">
       <formula1>"smiles,bpforms"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." errorStyle="warning" errorTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" showErrorMessage="1" showInputMessage="1" sqref="F3:F22"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="N3:N22"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="J3:J22"/>
-    <dataValidation allowBlank="0" error="Value must be an integer." errorStyle="warning" errorTitle="Charge" operator="between" prompt="Enter an integer." promptTitle="Charge" showErrorMessage="1" showInputMessage="1" sqref="H3:H22" type="whole">
+    <dataValidation sqref="F3:F22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Empirical formula" error="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Value must be an empirical formula (e.g. &quot;H2O&quot;)." promptTitle="Empirical formula" prompt="An empirical formula (e.g. 'H2O', 'CO2', or 'NaCl')&#10;&#10;Enter an empirical formula (e.g. &quot;H2O&quot;)." errorStyle="warning"/>
+    <dataValidation sqref="N3:N22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="J3:J22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="H3:H22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Charge" error="Value must be an integer." promptTitle="Charge" prompt="Enter an integer." type="whole" errorStyle="warning" operator="between">
       <formula1>-32768</formula1>
       <formula2>32767</formula2>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Value" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" showErrorMessage="1" showInputMessage="1" sqref="C3:C22" type="textLength">
+    <dataValidation sqref="C3:C22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Value" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Value" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Molecular weight" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Molecular weight" showErrorMessage="1" showInputMessage="1" sqref="G3:G22" type="decimal">
+    <dataValidation sqref="G3:G22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Molecular weight" error="Value must be a float or blank." promptTitle="Molecular weight" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B3:B22" type="textLength">
+    <dataValidation sqref="B3:B22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." errorStyle="warning" errorTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" showErrorMessage="1" showInputMessage="1" sqref="E3:E22" type="list">
+    <dataValidation sqref="E3:E22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Alphabet" error="Value must be one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." promptTitle="Alphabet" prompt="Select one of &quot;dna&quot;, &quot;rna&quot;, &quot;protein&quot;, &quot;canonical_dna&quot;, &quot;canonical_rna&quot;, &quot;canonical_protein&quot; or blank." type="list" errorStyle="warning">
       <formula1>"dna,rna,protein,canonical_dna,canonical_rna,canonical_protein"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." errorStyle="warning" errorTitle="Id" operator="between" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A3:A22" type="textLength">
+    <dataValidation sqref="A3:A22" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10; ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value mu ..." type="textLength" errorStyle="warning" operator="between">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -8600,21 +8600,21 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="10" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="11" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="10"/>
+    <col hidden="1" width="9" customWidth="1" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='Species' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='Species' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -9233,30 +9233,30 @@
   </sheetData>
   <autoFilter ref="A1:J21"/>
   <dataValidations count="10">
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="H2:H21"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="G2:G21"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="I2:I21" type="textLength">
+    <dataValidation sqref="H2:H21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="G2:G21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="I2:I21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Compartments:A&quot;." errorStyle="warning" errorTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." promptTitle="Compartment" showErrorMessage="1" showInputMessage="1" sqref="D2:D21" type="list">
+    <dataValidation sqref="D2:D21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Compartment" error="Value must be a value from &quot;Compartments:A&quot;." promptTitle="Compartment" prompt="Select a value from &quot;Compartments:A&quot;." type="list" errorStyle="warning">
       <formula1>Compartments!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Species types:A&quot;." errorStyle="warning" errorTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." promptTitle="Species type" showErrorMessage="1" showInputMessage="1" sqref="C2:C21" type="list">
+    <dataValidation sqref="C2:C21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Species type" error="Value must be a value from &quot;Species types:A&quot;." promptTitle="Species type" prompt="Select a value from &quot;Species types:A&quot;." type="list" errorStyle="warning">
       <formula1>'Species types'!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="F2:F21"/>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="E2:E21" type="list">
+    <dataValidation sqref="F2:F21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="E2:E21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot; or blank." type="list" errorStyle="warning">
       <formula1>"molecule"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B21" type="textLength">
+    <dataValidation sqref="B2:B21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="J2:J21"/>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A21" type="textLength">
+    <dataValidation sqref="J2:J21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="A2:A21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
@@ -9270,21 +9270,21 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="9" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col customWidth="1" max="12" min="1" width="15.7083333333333"/>
-    <col customWidth="1" hidden="1" max="16384" min="13" width="9"/>
+    <col width="15.7083333333333" customWidth="1" min="1" max="12"/>
+    <col hidden="1" width="9" customWidth="1" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>!!ObjTables Type='Data' Id='DistributionInitConcentration' ObjTablesVersion='0.0.8'</t>
+          <t>!!ObjTables type='Data' id='DistributionInitConcentration' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
         </is>
       </c>
     </row>
@@ -9993,34 +9993,34 @@
   </sheetData>
   <autoFilter ref="A1:L21"/>
   <dataValidations count="12">
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." errorStyle="warning" errorTitle="Id" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" showErrorMessage="1" showInputMessage="1" sqref="A2:A21" type="textLength">
+    <dataValidation sqref="A2:A21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Id" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters.&#10;&#10;Value must be unique." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." errorStyle="warning" errorTitle="Comments" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" showErrorMessage="1" showInputMessage="1" sqref="K2:K21" type="textLength">
+    <dataValidation sqref="K2:K21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Comments" error="Value must be a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." promptTitle="Comments" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 4294967295 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>4294967295</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." errorStyle="warning" errorTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." promptTitle="Distribution" showErrorMessage="1" showInputMessage="1" sqref="D2:D21"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning" errorTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" showErrorMessage="1" showInputMessage="1" sqref="J2:J21"/>
-    <dataValidation allowBlank="0" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning" errorTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" showErrorMessage="1" showInputMessage="1" sqref="I2:I21"/>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning" errorTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" showErrorMessage="1" showInputMessage="1" sqref="L2:L21"/>
-    <dataValidation allowBlank="0" error="Value must be a value from &quot;Species:A&quot;." errorStyle="warning" errorTitle="Species" prompt="Select a value from &quot;Species:A&quot;." promptTitle="Species" showErrorMessage="1" showInputMessage="1" sqref="C2:C21" type="list">
+    <dataValidation sqref="D2:D21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Distribution" error="Value must be a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;W ..." promptTitle="Distribution" prompt="Enter a comma-separated list of WC ontology terms &quot;Dirichlet_distribution&quot;, &quot;Gumbel_distribution&quot;, &quot;Laplace_distribution&quot;, &quot;Pareto_distribution&quot;, &quot;Poisson_distribution&quot;, &quot;Rayleigh_distribution&quot;, &quot;Vonmises_distribution&quot;, &quot;Wald_distribution&quot;, &quot;Weibull_d ..." errorStyle="warning"/>
+    <dataValidation sqref="J2:J21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Conclusions" error="Value must be a comma-separated list of values from &quot;Conclusions:A&quot; or blank." promptTitle="Conclusions" prompt="Enter a comma-separated list of values from &quot;Conclusions:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="I2:I21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;.&#10;&#10;Examples:&#10;* Obs1(+, s=50, q=100); Obs2(-)&#10;* Obs3(~, s=90)&#10;* Obs4(+, q=30)" errorStyle="warning"/>
+    <dataValidation sqref="L2:L21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." errorStyle="warning"/>
+    <dataValidation sqref="C2:C21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Species" error="Value must be a value from &quot;Species:A&quot;." promptTitle="Species" prompt="Select a value from &quot;Species:A&quot;." type="list" errorStyle="warning">
       <formula1>Species!$A$2:$A$1048576</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning" errorTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" showErrorMessage="1" showInputMessage="1" sqref="H2:H21"/>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Standard deviation" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Standard deviation" showErrorMessage="1" showInputMessage="1" sqref="F2:F21" type="decimal">
+    <dataValidation sqref="H2:H21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces.&#10;&#10;Examples:&#10;* doi: 10.1016/j.tcb.2015.09.004&#10;* chebi: CHEBI:15377, kegg.compound: C00001" errorStyle="warning"/>
+    <dataValidation sqref="F2:F21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a float or blank." errorStyle="warning" errorTitle="Mean" operator="greaterThanOrEqual" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." promptTitle="Mean" showErrorMessage="1" showInputMessage="1" sqref="E2:E21" type="decimal">
+    <dataValidation sqref="E2:E21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank.&#10;&#10;Value must be greater than or equal to 0.0." type="decimal" errorStyle="warning" operator="greaterThanOrEqual">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." errorStyle="warning" errorTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" showErrorMessage="1" showInputMessage="1" sqref="G2:G21" type="list">
+    <dataValidation sqref="G2:G21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')&#10;&#10;Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." type="list" errorStyle="warning">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." errorStyle="warning" errorTitle="Name" operator="lessThanOrEqual" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" showErrorMessage="1" showInputMessage="1" sqref="B2:B21" type="textLength">
+    <dataValidation sqref="B2:B21" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Name" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." type="textLength" errorStyle="warning" operator="lessThanOrEqual">
       <formula1>255</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>